<commit_message>
Write DynamicModel buffers during Update rather than Draw. Fix skybox motion blur, for good this time. Add V-Sync setting.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>en</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Fullscreen Resolution</t>
+  </si>
+  <si>
+    <t>vsync enabled</t>
+  </si>
+  <si>
+    <t>V-Sync Enabled</t>
   </si>
   <si>
     <t>gamma</t>
@@ -601,10 +607,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -984,19 +990,19 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="4" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1040,19 +1046,19 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="4" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1112,19 +1118,19 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="4" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1152,7 +1158,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>134</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>136</v>
       </c>
@@ -1214,6 +1220,14 @@
       </c>
       <c r="B75" s="1" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Localize shadow and boolean menu options. Fix a bug that allowed invalid values for the shadow setting.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t>en</t>
   </si>
@@ -163,10 +163,10 @@
     <t>Fullscreen Resolution</t>
   </si>
   <si>
-    <t>vsync enabled</t>
-  </si>
-  <si>
-    <t>V-Sync Enabled</t>
+    <t>vsync</t>
+  </si>
+  <si>
+    <t>V-Sync</t>
   </si>
   <si>
     <t>gamma</t>
@@ -187,16 +187,28 @@
     <t>Motion Blur Amount</t>
   </si>
   <si>
-    <t>reflections enabled</t>
-  </si>
-  <si>
-    <t>Reflections Enabled</t>
-  </si>
-  <si>
-    <t>bloom enabled</t>
-  </si>
-  <si>
-    <t>Bloom Enabled</t>
+    <t>reflections</t>
+  </si>
+  <si>
+    <t>Reflections</t>
+  </si>
+  <si>
+    <t>bloom</t>
+  </si>
+  <si>
+    <t>Bloom</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>On</t>
   </si>
   <si>
     <t>dynamic shadows</t>
@@ -205,6 +217,30 @@
     <t>Dynamic Shadows</t>
   </si>
   <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>ultra</t>
+  </si>
+  <si>
+    <t>Ultra</t>
+  </si>
+  <si>
     <t>controls</t>
   </si>
   <si>
@@ -473,6 +509,12 @@
   </si>
   <si>
     <t>No service</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -607,10 +649,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -998,11 +1040,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1046,19 +1088,19 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="1" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1102,11 +1144,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="4" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1126,11 +1168,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="1" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1166,7 +1208,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>136</v>
       </c>
@@ -1174,11 +1216,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="4" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1214,7 +1256,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>148</v>
       </c>
@@ -1228,6 +1270,62 @@
       </c>
       <c r="B76" s="1" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add option for high-resolution color/lighting.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>en</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>Reflections</t>
+  </si>
+  <si>
+    <t>high-res lighting</t>
+  </si>
+  <si>
+    <t>High-resolution color</t>
   </si>
   <si>
     <t>bloom</t>
@@ -649,10 +655,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1088,19 +1094,19 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="4" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1144,19 +1150,19 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="4" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1216,19 +1222,19 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1256,7 +1262,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>148</v>
       </c>
@@ -1264,7 +1270,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>150</v>
       </c>
@@ -1326,6 +1332,14 @@
       </c>
       <c r="B83" s="1" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove high-res lighting option. Add Entity OnSave command. Support for dynamic maps emerging from the fog.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>en</t>
   </si>
@@ -191,12 +191,6 @@
   </si>
   <si>
     <t>Reflections</t>
-  </si>
-  <si>
-    <t>high-res lighting</t>
-  </si>
-  <si>
-    <t>High-resolution color</t>
   </si>
   <si>
     <t>ambient occlusion</t>
@@ -661,10 +655,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1108,19 +1102,19 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="1" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1164,19 +1158,19 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1236,19 +1230,19 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="1" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1276,7 +1270,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>150</v>
       </c>
@@ -1284,7 +1278,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>152</v>
       </c>
@@ -1348,16 +1342,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048576">
+  <conditionalFormatting sqref="C2:C1048575">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Better phone and note animations. Player model now has three separate materials. Input binding localization.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="316">
   <si>
     <t>en</t>
   </si>
@@ -521,6 +521,450 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>LeftMouseButton</t>
+  </si>
+  <si>
+    <t>Left Mouse Button</t>
+  </si>
+  <si>
+    <t>MiddleMouseButton</t>
+  </si>
+  <si>
+    <t>Middle Mouse Button</t>
+  </si>
+  <si>
+    <t>RightMouseButton</t>
+  </si>
+  <si>
+    <t>Right Mouse Button</t>
+  </si>
+  <si>
+    <t>DPadUp</t>
+  </si>
+  <si>
+    <t>D-Pad Up</t>
+  </si>
+  <si>
+    <t>DPadDown</t>
+  </si>
+  <si>
+    <t>D-Pad Down</t>
+  </si>
+  <si>
+    <t>DPadLeft</t>
+  </si>
+  <si>
+    <t>D-Pad Left</t>
+  </si>
+  <si>
+    <t>DPadRight</t>
+  </si>
+  <si>
+    <t>D-Pad Right</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>LeftStick</t>
+  </si>
+  <si>
+    <t>Left Thumbstick Click</t>
+  </si>
+  <si>
+    <t>RightStick</t>
+  </si>
+  <si>
+    <t>Right Thumbstick Click</t>
+  </si>
+  <si>
+    <t>LeftShoulder</t>
+  </si>
+  <si>
+    <t>Left Shoulder</t>
+  </si>
+  <si>
+    <t>RightShoulder</t>
+  </si>
+  <si>
+    <t>Right Shoulder</t>
+  </si>
+  <si>
+    <t>LeftThumbstickLeft</t>
+  </si>
+  <si>
+    <t>Left Thumbstick Left</t>
+  </si>
+  <si>
+    <t>RightTrigger</t>
+  </si>
+  <si>
+    <t>Right Trigger</t>
+  </si>
+  <si>
+    <t>LeftTrigger</t>
+  </si>
+  <si>
+    <t>Left Trigger</t>
+  </si>
+  <si>
+    <t>RightThumbstickUp</t>
+  </si>
+  <si>
+    <t>Right Thumbstick Up</t>
+  </si>
+  <si>
+    <t>RightThumbstickDown</t>
+  </si>
+  <si>
+    <t>Right Thumbstick Down</t>
+  </si>
+  <si>
+    <t>RightThumbstickRight</t>
+  </si>
+  <si>
+    <t>Right Thumbstick Right</t>
+  </si>
+  <si>
+    <t>RightThumbstickLeft</t>
+  </si>
+  <si>
+    <t>Right Thumbstick Left</t>
+  </si>
+  <si>
+    <t>LeftThumbstickUp</t>
+  </si>
+  <si>
+    <t>Left Thumbstick Up</t>
+  </si>
+  <si>
+    <t>LeftThumbstickDown</t>
+  </si>
+  <si>
+    <t>Left Thumbstick Down</t>
+  </si>
+  <si>
+    <t>LeftThumbstickRight</t>
+  </si>
+  <si>
+    <t>Left Thumbstick Right</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>CapsLock</t>
+  </si>
+  <si>
+    <t>Capslock</t>
+  </si>
+  <si>
+    <t>Kana</t>
+  </si>
+  <si>
+    <t>Kanji</t>
+  </si>
+  <si>
+    <t>Escape</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>Spacebar</t>
+  </si>
+  <si>
+    <t>PageUp</t>
+  </si>
+  <si>
+    <t>Page Up</t>
+  </si>
+  <si>
+    <t>PageDown</t>
+  </si>
+  <si>
+    <t>Page Down</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>LeftWindows</t>
+  </si>
+  <si>
+    <t>Left Windows Key</t>
+  </si>
+  <si>
+    <t>RightWindows</t>
+  </si>
+  <si>
+    <t>Right Windows Key</t>
+  </si>
+  <si>
+    <t>NumPad0</t>
+  </si>
+  <si>
+    <t>Numpad 0</t>
+  </si>
+  <si>
+    <t>NumPad1</t>
+  </si>
+  <si>
+    <t>Numpad 1</t>
+  </si>
+  <si>
+    <t>NumPad2</t>
+  </si>
+  <si>
+    <t>Numpad 2</t>
+  </si>
+  <si>
+    <t>NumPad3</t>
+  </si>
+  <si>
+    <t>Numpad 3</t>
+  </si>
+  <si>
+    <t>NumPad4</t>
+  </si>
+  <si>
+    <t>Numpad 4</t>
+  </si>
+  <si>
+    <t>NumPad5</t>
+  </si>
+  <si>
+    <t>Numpad 5</t>
+  </si>
+  <si>
+    <t>NumPad6</t>
+  </si>
+  <si>
+    <t>Numpad 6</t>
+  </si>
+  <si>
+    <t>NumPad7</t>
+  </si>
+  <si>
+    <t>Numpad 7</t>
+  </si>
+  <si>
+    <t>NumPad8</t>
+  </si>
+  <si>
+    <t>Numpad 8</t>
+  </si>
+  <si>
+    <t>NumPad9</t>
+  </si>
+  <si>
+    <t>Numpad 9</t>
+  </si>
+  <si>
+    <t>Multiply</t>
+  </si>
+  <si>
+    <t>Numpad *</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Numpad +</t>
+  </si>
+  <si>
+    <t>Subtract</t>
+  </si>
+  <si>
+    <t>Numpad -</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Numpad .</t>
+  </si>
+  <si>
+    <t>Divide</t>
+  </si>
+  <si>
+    <t>Numpad /</t>
+  </si>
+  <si>
+    <t>OemClear</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>NumLock</t>
+  </si>
+  <si>
+    <t>LeftShift</t>
+  </si>
+  <si>
+    <t>Left Shift</t>
+  </si>
+  <si>
+    <t>RightShift</t>
+  </si>
+  <si>
+    <t>Right Shift</t>
+  </si>
+  <si>
+    <t>LeftControl</t>
+  </si>
+  <si>
+    <t>Left Control</t>
+  </si>
+  <si>
+    <t>RightControl</t>
+  </si>
+  <si>
+    <t>Right Control</t>
+  </si>
+  <si>
+    <t>LeftAlt</t>
+  </si>
+  <si>
+    <t>Left Alt</t>
+  </si>
+  <si>
+    <t>RightAlt</t>
+  </si>
+  <si>
+    <t>Right Alt</t>
+  </si>
+  <si>
+    <t>OemBackslash</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>OemSemicolon</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>OemPipe</t>
+  </si>
+  <si>
+    <t>OemPeriod</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>OemComma</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>OemQuestion</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>OemQuotes</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>OemOpenBrackets</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>OemCloseBrackets</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>OemPlus</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>OemMinus</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>OemTilde</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -655,10 +1099,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C173"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A126" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A145" activeCellId="0" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1342,8 +1786,720 @@
         <v>167</v>
       </c>
     </row>
+    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B127" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B128" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="B129" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B130" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="B131" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B132" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="B133" s="1" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B134" s="1" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="B135" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="B136" s="1" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048575">
+  <conditionalFormatting sqref="C2:C1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
God rays. Better textures. Less dizzying camera lean.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="318">
   <si>
     <t>en</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>Ambient occlusion</t>
+  </si>
+  <si>
+    <t>god rays</t>
+  </si>
+  <si>
+    <t>God rays</t>
   </si>
   <si>
     <t>bloom</t>
@@ -1099,10 +1105,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C173"/>
+  <dimension ref="A1:C174"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A126" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A145" activeCellId="0" sqref="A145"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1546,19 +1552,19 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1602,19 +1608,19 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="4" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1674,19 +1680,19 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="4" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1714,7 +1720,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>150</v>
       </c>
@@ -1722,7 +1728,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>152</v>
       </c>
@@ -1847,23 +1853,23 @@
         <v>182</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>29</v>
+        <v>184</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>29</v>
+        <v>184</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>183</v>
+        <v>29</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>184</v>
+        <v>29</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1922,11 +1928,11 @@
         <v>198</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="1" t="s">
         <v>200</v>
       </c>
     </row>
@@ -1970,33 +1976,33 @@
         <v>210</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>211</v>
+      <c r="B108" s="0" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>215</v>
@@ -2007,28 +2013,28 @@
         <v>216</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>220</v>
@@ -2055,159 +2061,159 @@
         <v>225</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="B127" s="1" t="n">
-        <v>0</v>
+        <v>235</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B128" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B129" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B130" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B131" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B132" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B133" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B134" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="B137" s="1" t="s">
         <v>245</v>
+      </c>
+      <c r="B137" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,25 +2344,25 @@
         <v>277</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="B154" s="0" t="s">
+      <c r="B154" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="B155" s="1" t="s">
-        <v>280</v>
+      <c r="B155" s="0" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>282</v>
@@ -2423,15 +2429,15 @@
         <v>297</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,6 +2502,14 @@
       </c>
       <c r="B173" s="1" t="s">
         <v>315</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring for readability. Sound pausing and volume controls.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="322">
   <si>
     <t>en</t>
   </si>
@@ -251,6 +251,18 @@
   </si>
   <si>
     <t>Ultra</t>
+  </si>
+  <si>
+    <t>sound effect volume</t>
+  </si>
+  <si>
+    <t>Sound Effect Volume</t>
+  </si>
+  <si>
+    <t>music volume</t>
+  </si>
+  <si>
+    <t>Music Volume</t>
   </si>
   <si>
     <t>controls</t>
@@ -1105,10 +1117,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C174"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1560,11 +1572,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="1" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1576,11 +1588,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="4" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1616,11 +1628,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1632,11 +1644,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="4" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1688,11 +1700,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="1" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1704,11 +1716,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="4" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1728,7 +1740,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>152</v>
       </c>
@@ -1744,7 +1756,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>156</v>
       </c>
@@ -1861,31 +1873,31 @@
         <v>184</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>29</v>
+        <v>186</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>29</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>187</v>
+        <v>29</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>188</v>
+        <v>29</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1936,19 +1948,19 @@
         <v>200</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="B104" s="0" t="s">
+      <c r="B104" s="1" t="s">
         <v>204</v>
       </c>
     </row>
@@ -1984,73 +1996,73 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>224</v>
@@ -2069,167 +2081,167 @@
         <v>227</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="B128" s="1" t="n">
-        <v>0</v>
+        <v>238</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="B129" s="1" t="n">
-        <v>1</v>
+        <v>239</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B130" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B131" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B132" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B133" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B134" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B137" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
+      </c>
+      <c r="B138" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="B139" s="1" t="s">
         <v>249</v>
+      </c>
+      <c r="B139" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2352,11 +2364,11 @@
         <v>279</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="B155" s="0" t="s">
+      <c r="B155" s="1" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2365,20 +2377,20 @@
         <v>282</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="B157" s="1" t="s">
         <v>284</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>286</v>
@@ -2437,23 +2449,23 @@
         <v>299</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,6 +2522,22 @@
       </c>
       <c r="B174" s="1" t="s">
         <v>317</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix player data not being persisted between maps. Fix some issues with the vault. Fix a crash on the start map. Re-map slow-motion to a separate "special ability" button.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="324">
   <si>
     <t>en</t>
   </si>
@@ -335,6 +335,12 @@
   </si>
   <si>
     <t>Roll / Kick</t>
+  </si>
+  <si>
+    <t>special ability</t>
+  </si>
+  <si>
+    <t>Special Ability</t>
   </si>
   <si>
     <t>toggle phone</t>
@@ -1117,10 +1123,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1588,19 +1594,19 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="4" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1644,19 +1650,19 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1716,19 +1722,19 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="4" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1756,7 +1762,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>156</v>
       </c>
@@ -1764,7 +1770,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>158</v>
       </c>
@@ -1889,23 +1895,23 @@
         <v>188</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>29</v>
+        <v>190</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>29</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>189</v>
+        <v>29</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>190</v>
+        <v>29</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1964,11 +1970,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="1" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2012,33 +2018,33 @@
         <v>216</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>217</v>
+      <c r="B111" s="0" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>221</v>
@@ -2049,28 +2055,28 @@
         <v>222</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>226</v>
@@ -2097,159 +2103,159 @@
         <v>231</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="B130" s="1" t="n">
-        <v>0</v>
+        <v>241</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B131" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B132" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B133" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B134" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B137" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B138" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="B140" s="1" t="s">
         <v>251</v>
+      </c>
+      <c r="B140" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2380,25 +2386,25 @@
         <v>283</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="B157" s="0" t="s">
+      <c r="B157" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="B158" s="1" t="s">
-        <v>286</v>
+      <c r="B158" s="0" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>288</v>
@@ -2465,15 +2471,15 @@
         <v>303</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2538,6 +2544,14 @@
       </c>
       <c r="B176" s="1" t="s">
         <v>321</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add power sound. Slight improvement to propagator performance. UI text elements now have interpolation disabled in the editor. Sound update. Finally fix an old slider bug where the direction was sometimes reversed. Re-order levels.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -41,16 +41,16 @@
     <t>3 | Dawn</t>
   </si>
   <si>
+    <t>map forest</t>
+  </si>
+  <si>
+    <t>4 | Forest</t>
+  </si>
+  <si>
     <t>map monolith</t>
   </si>
   <si>
-    <t>4 | Monolith</t>
-  </si>
-  <si>
-    <t>map forest</t>
-  </si>
-  <si>
-    <t>5 | Forest</t>
+    <t>5 | Monolith</t>
   </si>
   <si>
     <t>map valley</t>
@@ -1121,12 +1121,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C177"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2555,7 +2556,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048576">
+  <conditionalFormatting sqref="C2:C1048575">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
AmbientSound. Collectibles keep track of how many you've got. Rift sounds. Fix TimeTrialUI save crash.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="326">
   <si>
     <t>en</t>
   </si>
@@ -533,6 +533,12 @@
   </si>
   <si>
     <t>{0} / {1} notes read</t>
+  </si>
+  <si>
+    <t>orbs collected</t>
+  </si>
+  <si>
+    <t>{0} orbs collected</t>
   </si>
   <si>
     <t>no service</t>
@@ -1121,13 +1127,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:C178"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1904,23 +1910,23 @@
         <v>190</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>191</v>
+        <v>29</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>192</v>
+        <v>29</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1979,11 +1985,11 @@
         <v>206</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="B106" s="0" t="s">
+      <c r="B106" s="1" t="s">
         <v>208</v>
       </c>
     </row>
@@ -2027,33 +2033,33 @@
         <v>218</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>219</v>
+      <c r="B112" s="0" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>223</v>
@@ -2064,28 +2070,28 @@
         <v>224</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>228</v>
@@ -2112,159 +2118,159 @@
         <v>233</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="B131" s="1" t="n">
-        <v>0</v>
+        <v>243</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B132" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B133" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B134" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B137" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B138" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B141" s="1" t="s">
         <v>253</v>
+      </c>
+      <c r="B141" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2395,25 +2401,25 @@
         <v>285</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="B158" s="0" t="s">
+      <c r="B158" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>288</v>
+      <c r="B159" s="0" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>290</v>
@@ -2480,15 +2486,15 @@
         <v>305</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2555,8 +2561,16 @@
         <v>323</v>
       </c>
     </row>
+    <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048575">
+  <conditionalFormatting sqref="C2:C1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Remove old EditorUI. Use ulong GUIDs rather than human-readable string IDs.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="324">
   <si>
     <t>en</t>
   </si>
@@ -509,12 +509,6 @@
   </si>
   <si>
     <t>Saved</t>
-  </si>
-  <si>
-    <t>editor menu</t>
-  </si>
-  <si>
-    <t>[Space] – Show menu</t>
   </si>
   <si>
     <t>compose</t>
@@ -1130,10 +1124,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
+      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1910,23 +1904,23 @@
         <v>190</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>192</v>
+        <v>29</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>192</v>
+        <v>29</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>29</v>
+        <v>191</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1985,11 +1979,11 @@
         <v>206</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="0" t="s">
         <v>208</v>
       </c>
     </row>
@@ -2033,33 +2027,33 @@
         <v>218</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B112" s="0" t="s">
-        <v>220</v>
+      <c r="B112" s="1" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>223</v>
@@ -2070,28 +2064,28 @@
         <v>224</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>228</v>
@@ -2118,159 +2112,159 @@
         <v>233</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
+      </c>
+      <c r="B131" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B132" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B133" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B134" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B137" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B138" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="B141" s="1" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2401,25 +2395,25 @@
         <v>285</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="B158" s="0" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B159" s="0" t="s">
-        <v>289</v>
+      <c r="B159" s="1" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>290</v>
@@ -2486,15 +2480,15 @@
         <v>305</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B169" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2561,16 +2555,8 @@
         <v>323</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048576">
+  <conditionalFormatting sqref="C2:C1048575">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Improve scroll buttons on the main menu.
bug 18:closed
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="323">
   <si>
     <t>en</t>
   </si>
@@ -146,27 +146,22 @@
     <t>modify setting</t>
   </si>
   <si>
-    <t>Scroll or click to modify
-[{{ToggleFullscreen}}] to toggle fullscreen</t>
+    <t>[{{ToggleFullscreen}}] to toggle fullscreen</t>
   </si>
   <si>
     <t>modify setting gamepad</t>
   </si>
   <si>
-    <t>[A] or [LeftStick] to modify
-[{{ToggleFullscreen}}] to toggle fullscreen</t>
-  </si>
-  <si>
     <t>fullscreen resolution</t>
   </si>
   <si>
-    <t>Fullscreen Resolution</t>
+    <t>Resolution</t>
   </si>
   <si>
     <t>vsync</t>
   </si>
   <si>
-    <t>V-Sync</t>
+    <t>V-sync</t>
   </si>
   <si>
     <t>gamma</t>
@@ -178,13 +173,13 @@
     <t>field of view</t>
   </si>
   <si>
-    <t>Field of View</t>
+    <t>Field of view</t>
   </si>
   <si>
     <t>motion blur amount</t>
   </si>
   <si>
-    <t>Motion Blur Amount</t>
+    <t>Motion blur</t>
   </si>
   <si>
     <t>reflections</t>
@@ -226,7 +221,7 @@
     <t>dynamic shadows</t>
   </si>
   <si>
-    <t>Dynamic Shadows</t>
+    <t>Shadows</t>
   </si>
   <si>
     <t>low</t>
@@ -256,13 +251,13 @@
     <t>sound effect volume</t>
   </si>
   <si>
-    <t>Sound Effect Volume</t>
+    <t>SFX volume</t>
   </si>
   <si>
     <t>music volume</t>
   </si>
   <si>
-    <t>Music Volume</t>
+    <t>Music volume</t>
   </si>
   <si>
     <t>controls</t>
@@ -280,43 +275,43 @@
     <t>invert look x</t>
   </si>
   <si>
-    <t>Invert Look X</t>
+    <t>Invert look X</t>
   </si>
   <si>
     <t>invert look y</t>
   </si>
   <si>
-    <t>Invert Look Y</t>
+    <t>Invert look Y</t>
   </si>
   <si>
     <t>look sensitivity</t>
   </si>
   <si>
-    <t>Look Sensitivity</t>
+    <t>Look sensitivity</t>
   </si>
   <si>
     <t>move forward</t>
   </si>
   <si>
-    <t>Move Forward</t>
+    <t>Move forward</t>
   </si>
   <si>
     <t>move left</t>
   </si>
   <si>
-    <t>Move Left</t>
+    <t>Move left</t>
   </si>
   <si>
     <t>move backward</t>
   </si>
   <si>
-    <t>Move Backward</t>
+    <t>Move backward</t>
   </si>
   <si>
     <t>move right</t>
   </si>
   <si>
-    <t>Move Right</t>
+    <t>Move right</t>
   </si>
   <si>
     <t>jump</t>
@@ -340,13 +335,13 @@
     <t>special ability</t>
   </si>
   <si>
-    <t>Special Ability</t>
+    <t>Special ability</t>
   </si>
   <si>
     <t>toggle phone</t>
   </si>
   <si>
-    <t>Toggle Phone</t>
+    <t>Toggle phone</t>
   </si>
   <si>
     <t>quicksave</t>
@@ -358,13 +353,13 @@
     <t>toggle fullscreen</t>
   </si>
   <si>
-    <t>Toggle Fullscreen</t>
+    <t>Toggle fullscreen</t>
   </si>
   <si>
     <t>new game</t>
   </si>
   <si>
-    <t>New Game</t>
+    <t>New game</t>
   </si>
   <si>
     <t>alpha disclaimer</t>
@@ -460,7 +455,7 @@
     <t>main menu</t>
   </si>
   <si>
-    <t>Main Menu</t>
+    <t>Main menu</t>
   </si>
   <si>
     <t>quit prompt</t>
@@ -1126,8 +1121,8 @@
   </sheetPr>
   <dimension ref="A1:C177"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1307,7 +1302,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>42</v>
       </c>
@@ -1315,596 +1310,596 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,271 +1912,271 @@
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B106" s="0" t="s">
         <v>207</v>
-      </c>
-      <c r="B106" s="0" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B107" s="0" t="s">
         <v>209</v>
-      </c>
-      <c r="B107" s="0" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B108" s="0" t="s">
         <v>211</v>
-      </c>
-      <c r="B108" s="0" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B109" s="0" t="s">
         <v>213</v>
-      </c>
-      <c r="B109" s="0" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B110" s="0" t="s">
         <v>215</v>
-      </c>
-      <c r="B110" s="0" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B111" s="0" t="s">
         <v>217</v>
-      </c>
-      <c r="B111" s="0" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B131" s="1" t="n">
         <v>0</v>
@@ -2189,7 +2184,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B132" s="1" t="n">
         <v>1</v>
@@ -2197,7 +2192,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B133" s="1" t="n">
         <v>2</v>
@@ -2205,7 +2200,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B134" s="1" t="n">
         <v>3</v>
@@ -2213,7 +2208,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B135" s="1" t="n">
         <v>4</v>
@@ -2221,7 +2216,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B136" s="1" t="n">
         <v>5</v>
@@ -2229,7 +2224,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B137" s="1" t="n">
         <v>6</v>
@@ -2237,7 +2232,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B138" s="1" t="n">
         <v>7</v>
@@ -2245,7 +2240,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B139" s="1" t="n">
         <v>8</v>
@@ -2253,7 +2248,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B140" s="1" t="n">
         <v>9</v>
@@ -2261,298 +2256,298 @@
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B146" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B158" s="0" t="s">
         <v>286</v>
-      </c>
-      <c r="B158" s="0" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B163" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="B164" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B169" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B170" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B171" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B172" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B173" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B174" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B175" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B176" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B177" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Menu button to reset options to factory defaults.
bug 43:closed
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="329">
   <si>
     <t>en</t>
   </si>
@@ -141,6 +141,24 @@
   </si>
   <si>
     <t>O P T I O N S</t>
+  </si>
+  <si>
+    <t>reset options</t>
+  </si>
+  <si>
+    <t>Reset to factory defaults</t>
+  </si>
+  <si>
+    <t>reset options?</t>
+  </si>
+  <si>
+    <t>Reset to factory defaults and exit the game?</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>Reset and exit</t>
   </si>
   <si>
     <t>modify setting</t>
@@ -1119,10 +1137,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:C180"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1315,31 +1333,31 @@
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,11 +1616,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="1" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1622,11 +1640,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1654,11 +1672,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="1" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1678,11 +1696,11 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1726,11 +1744,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="1" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1750,11 +1768,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="4" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1766,7 +1784,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>157</v>
       </c>
@@ -1790,7 +1808,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>163</v>
       </c>
@@ -1899,39 +1917,39 @@
         <v>189</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>29</v>
+        <v>191</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>194</v>
+        <v>29</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>195</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,27 +1992,27 @@
         <v>205</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="B106" s="0" t="s">
+      <c r="B106" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B107" s="0" t="s">
+      <c r="B107" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="B108" s="0" t="s">
+      <c r="B108" s="1" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2022,81 +2040,81 @@
         <v>217</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>220</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>231</v>
@@ -2107,175 +2125,175 @@
         <v>232</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="B131" s="1" t="n">
-        <v>0</v>
+        <v>244</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="B132" s="1" t="n">
-        <v>1</v>
+        <v>245</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="B133" s="1" t="n">
-        <v>2</v>
+        <v>246</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B134" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B137" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B138" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
+      </c>
+      <c r="B141" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
+      </c>
+      <c r="B142" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="B143" s="1" t="s">
         <v>256</v>
+      </c>
+      <c r="B143" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2390,11 +2408,11 @@
         <v>284</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="B158" s="0" t="s">
+      <c r="B158" s="1" t="s">
         <v>286</v>
       </c>
     </row>
@@ -2403,28 +2421,28 @@
         <v>287</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="B161" s="1" t="s">
         <v>291</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>293</v>
@@ -2475,31 +2493,31 @@
         <v>304</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,8 +2568,32 @@
         <v>322</v>
       </c>
     </row>
+    <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048575">
+  <conditionalFormatting sqref="C2:C1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Settings menu is scrollable now. You can open the menu while the editor is active now. Starting work on GeeUI perf.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="331">
   <si>
     <t>en</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>Quicksave</t>
+  </si>
+  <si>
+    <t>toggle console</t>
+  </si>
+  <si>
+    <t>Toggle console</t>
   </si>
   <si>
     <t>toggle fullscreen</t>
@@ -1137,10 +1143,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C180"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1640,19 +1646,19 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="4" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1696,19 +1702,19 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="4" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1768,19 +1774,19 @@
         <v>152</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="4" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1808,7 +1814,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>163</v>
       </c>
@@ -1816,7 +1822,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>165</v>
       </c>
@@ -1941,23 +1947,23 @@
         <v>195</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>29</v>
+        <v>197</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>29</v>
+        <v>197</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>196</v>
+        <v>29</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>197</v>
+        <v>29</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,11 +2022,11 @@
         <v>211</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="1" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2064,33 +2070,33 @@
         <v>223</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>224</v>
+      <c r="B115" s="0" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>228</v>
@@ -2101,28 +2107,28 @@
         <v>229</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>233</v>
@@ -2149,159 +2155,159 @@
         <v>238</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="B134" s="1" t="n">
-        <v>0</v>
+        <v>248</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B137" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B138" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B141" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B142" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="B144" s="1" t="s">
         <v>258</v>
+      </c>
+      <c r="B144" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,25 +2438,25 @@
         <v>290</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="B161" s="0" t="s">
+      <c r="B161" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>293</v>
+      <c r="B162" s="0" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>295</v>
@@ -2517,15 +2523,15 @@
         <v>310</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2590,6 +2596,14 @@
       </c>
       <c r="B180" s="1" t="s">
         <v>328</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix player falling backward after top-out. Play top-out animation when the player is falling too fast and grabs a ledge. Fix the roll being enabled while phone or note is active. Fix moves being enabled in start map after picking up the note or phone. Remove ".map" from challenge menu. Hopefully fix some crashes related to FullscreenQuad and the UIRenderer scissor rectangle going outside the viewport during window resizes.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="339">
   <si>
     <t>en</t>
   </si>
@@ -474,6 +474,30 @@
   </si>
   <si>
     <t>C R E D I T S</t>
+  </si>
+  <si>
+    <t>challenge levels</t>
+  </si>
+  <si>
+    <t>Challenge Levels</t>
+  </si>
+  <si>
+    <t>challenge title</t>
+  </si>
+  <si>
+    <t>C H A L L E N G E</t>
+  </si>
+  <si>
+    <t>official levels</t>
+  </si>
+  <si>
+    <t>Official Levels</t>
+  </si>
+  <si>
+    <t>workshop levels</t>
+  </si>
+  <si>
+    <t>Workshop Levels</t>
   </si>
   <si>
     <t>main menu</t>
@@ -1143,10 +1167,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1782,11 +1806,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="1" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1814,15 +1838,15 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>165</v>
       </c>
@@ -1854,7 +1878,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>173</v>
       </c>
@@ -1955,47 +1979,47 @@
         <v>197</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>29</v>
+        <v>199</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>29</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>204</v>
+        <v>29</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>205</v>
+        <v>29</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2030,35 +2054,35 @@
         <v>213</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="B110" s="0" t="s">
+      <c r="B110" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B111" s="0" t="s">
+      <c r="B111" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B112" s="0" t="s">
+      <c r="B112" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="B113" s="0" t="s">
+      <c r="B113" s="1" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2078,268 +2102,268 @@
         <v>225</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="B116" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>228</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>230</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="B135" s="1" t="n">
-        <v>0</v>
+        <v>253</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="B136" s="1" t="n">
-        <v>1</v>
+        <v>254</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="B137" s="1" t="n">
-        <v>2</v>
+        <v>255</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B138" s="1" t="n">
-        <v>3</v>
+        <v>256</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B141" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B142" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B144" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
+      </c>
+      <c r="B145" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
+      </c>
+      <c r="B146" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
+      </c>
+      <c r="B147" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="B148" s="1" t="s">
         <v>266</v>
+      </c>
+      <c r="B148" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2446,11 +2470,11 @@
         <v>292</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="B162" s="0" t="s">
+      <c r="B162" s="1" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2459,36 +2483,36 @@
         <v>295</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="B166" s="1" t="s">
         <v>301</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>303</v>
@@ -2531,39 +2555,39 @@
         <v>312</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2604,6 +2628,38 @@
       </c>
       <c r="B181" s="1" t="s">
         <v>330</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix main menu fading. Add "demo mode". Mess with entity GUIDs again... maybe it works?
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="333">
   <si>
     <t>en</t>
   </si>
@@ -422,28 +422,10 @@
     <t>Load</t>
   </si>
   <si>
-    <t>sandbox</t>
-  </si>
-  <si>
-    <t>Sandbox</t>
-  </si>
-  <si>
-    <t>sandbox disclaimer</t>
-  </si>
-  <si>
-    <t>The sandbox is unpolished and has no tutorial. You may want to complete the game first.</t>
-  </si>
-  <si>
-    <t>play anyway</t>
-  </si>
-  <si>
-    <t>Play anyway</t>
-  </si>
-  <si>
-    <t>play anyway gamepad</t>
-  </si>
-  <si>
-    <t>[A] Play anyway</t>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>DEMO</t>
   </si>
   <si>
     <t>cheat</t>
@@ -1167,10 +1149,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
+      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1734,11 +1716,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="1" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1814,11 +1796,11 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="4" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1838,11 +1820,11 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="1" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1854,7 +1836,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>167</v>
       </c>
@@ -1878,7 +1860,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>173</v>
       </c>
@@ -1987,39 +1969,39 @@
         <v>199</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>201</v>
+        <v>29</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>202</v>
+        <v>29</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>29</v>
+        <v>204</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>29</v>
+        <v>205</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2062,27 +2044,27 @@
         <v>215</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="0" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="0" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="0" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2110,81 +2092,81 @@
         <v>227</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B117" s="0" t="s">
+      <c r="B117" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+      <c r="B118" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="B118" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="B119" s="0" t="s">
-        <v>233</v>
+      <c r="B119" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>241</v>
@@ -2195,175 +2177,175 @@
         <v>242</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
+      </c>
+      <c r="B136" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
+      </c>
+      <c r="B137" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
+      </c>
+      <c r="B138" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B141" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B142" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B144" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B145" s="1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="B146" s="1" t="n">
-        <v>7</v>
+        <v>261</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="B147" s="1" t="n">
-        <v>8</v>
+        <v>263</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="B148" s="1" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2478,11 +2460,11 @@
         <v>294</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" s="0" t="s">
         <v>296</v>
       </c>
     </row>
@@ -2491,28 +2473,28 @@
         <v>297</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B165" s="1" t="s">
+    </row>
+    <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0" t="s">
+      <c r="B166" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="B166" s="0" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>303</v>
@@ -2563,31 +2545,31 @@
         <v>314</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B174" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B175" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B176" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,32 +2620,8 @@
         <v>332</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048576">
+  <conditionalFormatting sqref="C2:C1048573">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Localize workshop map upload notifier.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="337">
   <si>
     <t>en</t>
   </si>
@@ -480,6 +480,18 @@
   </si>
   <si>
     <t>Workshop Levels</t>
+  </si>
+  <si>
+    <t>downloading workshop maps</t>
+  </si>
+  <si>
+    <t>Downloading {0} workshop maps...</t>
+  </si>
+  <si>
+    <t>workshop downloads complete</t>
+  </si>
+  <si>
+    <t>Workshop maps synced!</t>
   </si>
   <si>
     <t>main menu</t>
@@ -1149,10 +1161,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C184"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1796,11 +1808,11 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="1" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1812,11 +1824,11 @@
         <v>160</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="4" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1836,7 +1848,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>167</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>171</v>
       </c>
@@ -1969,31 +1981,31 @@
         <v>199</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>29</v>
+        <v>201</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>29</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>202</v>
+        <v>29</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>203</v>
+        <v>29</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2044,19 +2056,19 @@
         <v>215</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B111" s="0" t="s">
+      <c r="B111" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B112" s="0" t="s">
+      <c r="B112" s="1" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2092,73 +2104,73 @@
         <v>227</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>239</v>
@@ -2177,167 +2189,167 @@
         <v>242</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="B136" s="1" t="n">
-        <v>0</v>
+        <v>253</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B137" s="1" t="n">
-        <v>1</v>
+        <v>254</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B138" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B141" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B142" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B144" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B145" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
+      </c>
+      <c r="B146" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="B147" s="1" t="s">
         <v>264</v>
+      </c>
+      <c r="B147" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2460,11 +2472,11 @@
         <v>294</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="B163" s="0" t="s">
+      <c r="B163" s="1" t="s">
         <v>296</v>
       </c>
     </row>
@@ -2473,20 +2485,20 @@
         <v>297</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="B165" s="1" t="s">
         <v>299</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>301</v>
@@ -2545,23 +2557,23 @@
         <v>314</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,8 +2632,24 @@
         <v>332</v>
       </c>
     </row>
+    <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048573">
+  <conditionalFormatting sqref="C2:C1048575">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add optional reticle. It is now impossible to spawn below a lower limit. Demo mode works correctly alongside the normal "new game" functionality. Run animation speed is faster now. Reverse wall-slide is gone.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="339">
   <si>
     <t>en</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Reflections</t>
+  </si>
+  <si>
+    <t>reticle</t>
+  </si>
+  <si>
+    <t>Reticle</t>
   </si>
   <si>
     <t>ambient occlusion</t>
@@ -1161,10 +1167,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1672,19 +1678,19 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="4" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1824,19 +1830,19 @@
         <v>160</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="4" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1864,7 +1870,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>171</v>
       </c>
@@ -1872,7 +1878,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>173</v>
       </c>
@@ -1997,23 +2003,23 @@
         <v>203</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>29</v>
+        <v>205</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>29</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>204</v>
+        <v>29</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>205</v>
+        <v>29</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2072,11 +2078,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="B113" s="0" t="s">
+      <c r="B113" s="1" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2120,33 +2126,33 @@
         <v>231</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>232</v>
+      <c r="B119" s="0" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>236</v>
@@ -2157,28 +2163,28 @@
         <v>237</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>241</v>
@@ -2205,159 +2211,159 @@
         <v>246</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="B138" s="1" t="n">
-        <v>0</v>
+        <v>256</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B141" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B142" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B144" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B145" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B146" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B147" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="B148" s="1" t="s">
         <v>266</v>
+      </c>
+      <c r="B148" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,25 +2494,25 @@
         <v>298</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="B165" s="0" t="s">
+      <c r="B165" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="B166" s="1" t="s">
-        <v>301</v>
+      <c r="B166" s="0" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>303</v>
@@ -2573,15 +2579,15 @@
         <v>318</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2648,8 +2654,16 @@
         <v>336</v>
       </c>
     </row>
+    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048575">
+  <conditionalFormatting sqref="C2:C1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fix menu toggle in editor. Improve snow effects. Fix the cloud texture. Again.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="341">
   <si>
     <t>en</t>
   </si>
@@ -53,10 +53,16 @@
     <t>5 | Monolith</t>
   </si>
   <si>
+    <t>map fracture</t>
+  </si>
+  <si>
+    <t>6 | Fracture</t>
+  </si>
+  <si>
     <t>map valley</t>
   </si>
   <si>
-    <t>6 | Valley</t>
+    <t>7 | Valley</t>
   </si>
   <si>
     <t>toggle fullscreen tooltip</t>
@@ -1167,10 +1173,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1242,7 +1248,7 @@
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1250,7 +1256,7 @@
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1387,15 +1393,15 @@
         <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,19 +1692,19 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="4" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1838,19 +1844,19 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="4" t="s">
         <v>166</v>
       </c>
     </row>
@@ -1878,7 +1884,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>173</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>175</v>
       </c>
@@ -2011,23 +2017,23 @@
         <v>205</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>29</v>
+        <v>207</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>29</v>
+        <v>207</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>206</v>
+        <v>31</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>207</v>
+        <v>31</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,11 +2092,11 @@
         <v>221</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="B114" s="0" t="s">
+      <c r="B114" s="1" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2134,33 +2140,33 @@
         <v>233</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>234</v>
+      <c r="B120" s="0" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>238</v>
@@ -2171,28 +2177,28 @@
         <v>239</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>243</v>
@@ -2219,159 +2225,159 @@
         <v>248</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="B139" s="1" t="n">
-        <v>0</v>
+        <v>258</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B141" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B142" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B144" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B145" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B146" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B147" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B148" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="B149" s="1" t="s">
         <v>268</v>
+      </c>
+      <c r="B149" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,25 +2508,25 @@
         <v>300</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="B166" s="0" t="s">
+      <c r="B166" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>303</v>
+      <c r="B167" s="0" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>305</v>
@@ -2587,15 +2593,15 @@
         <v>320</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,6 +2666,14 @@
       </c>
       <c r="B185" s="1" t="s">
         <v>338</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved borderless fullscreen window support.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="347">
   <si>
     <t>en</t>
   </si>
@@ -180,6 +180,24 @@
   </si>
   <si>
     <t>Resolution</t>
+  </si>
+  <si>
+    <t>borderless</t>
+  </si>
+  <si>
+    <t>Borderless window</t>
+  </si>
+  <si>
+    <t>apply resolution</t>
+  </si>
+  <si>
+    <t>Apply resolution</t>
+  </si>
+  <si>
+    <t>enter fullscreen</t>
+  </si>
+  <si>
+    <t>Enter fullscreen [{{ToggleFullscreen}}]</t>
   </si>
   <si>
     <t>vsync</t>
@@ -1173,10 +1191,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C189"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1700,11 +1718,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="1" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1724,11 +1742,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="4" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1852,11 +1870,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="1" t="s">
         <v>166</v>
       </c>
     </row>
@@ -1876,11 +1894,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="4" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1892,7 +1910,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>175</v>
       </c>
@@ -1916,7 +1934,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>181</v>
       </c>
@@ -2025,39 +2043,39 @@
         <v>207</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>31</v>
+        <v>209</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>212</v>
+        <v>31</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>213</v>
+        <v>31</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,27 +2118,27 @@
         <v>223</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="B115" s="0" t="s">
+      <c r="B115" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="B116" s="0" t="s">
+      <c r="B116" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B117" s="0" t="s">
+      <c r="B117" s="1" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2148,81 +2166,81 @@
         <v>235</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>238</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>249</v>
@@ -2233,175 +2251,175 @@
         <v>250</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="B140" s="1" t="n">
-        <v>0</v>
+        <v>262</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="B141" s="1" t="n">
-        <v>1</v>
+        <v>263</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="B142" s="1" t="n">
-        <v>2</v>
+        <v>264</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B144" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B145" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B146" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B147" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B148" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B149" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
+      </c>
+      <c r="B150" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
+      </c>
+      <c r="B151" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="B152" s="1" t="s">
         <v>274</v>
+      </c>
+      <c r="B152" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2516,11 +2534,11 @@
         <v>302</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="B167" s="0" t="s">
+      <c r="B167" s="1" t="s">
         <v>304</v>
       </c>
     </row>
@@ -2529,28 +2547,28 @@
         <v>305</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="B170" s="1" t="s">
         <v>309</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>311</v>
@@ -2601,31 +2619,31 @@
         <v>322</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2674,6 +2692,30 @@
       </c>
       <c r="B186" s="1" t="s">
         <v>340</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cloud shadows. Phone UI indicator when Mark is typing. Display note and orb count when loading a new map.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="358">
   <si>
     <t>en</t>
   </si>
@@ -578,6 +578,9 @@
     <t>Saved</t>
   </si>
   <si>
+    <t>...</t>
+  </si>
+  <si>
     <t>compose</t>
   </si>
   <si>
@@ -590,10 +593,40 @@
     <t>[A] Compose</t>
   </si>
   <si>
+    <t>one note</t>
+  </si>
+  <si>
+    <t>1 note</t>
+  </si>
+  <si>
+    <t>note count</t>
+  </si>
+  <si>
+    <t>{0} notes</t>
+  </si>
+  <si>
     <t>notes read</t>
   </si>
   <si>
     <t>{0} / {1} notes read</t>
+  </si>
+  <si>
+    <t>one orb</t>
+  </si>
+  <si>
+    <t>1 orb</t>
+  </si>
+  <si>
+    <t>orb count</t>
+  </si>
+  <si>
+    <t>{0} orbs</t>
+  </si>
+  <si>
+    <t>one orb collected</t>
+  </si>
+  <si>
+    <t>1 orb collected</t>
   </si>
   <si>
     <t>orbs collected</t>
@@ -1191,10 +1224,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C189"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1963,108 +1996,108 @@
         <v>187</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>213</v>
@@ -2072,503 +2105,503 @@
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>31</v>
+        <v>214</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>31</v>
+        <v>215</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>224</v>
+        <v>31</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>225</v>
+        <v>31</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B117" s="1" t="s">
+    </row>
+    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+      <c r="B118" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B118" s="0" t="s">
+    </row>
+    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+      <c r="B119" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B119" s="0" t="s">
+    </row>
+    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+      <c r="B120" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B120" s="0" t="s">
+    </row>
+    <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="B121" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B121" s="0" t="s">
+    </row>
+    <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="B122" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B122" s="0" t="s">
+    </row>
+    <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+      <c r="B123" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B123" s="0" t="s">
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="B124" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>245</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>247</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>249</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="B143" s="1" t="n">
-        <v>0</v>
+        <v>270</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="B144" s="1" t="n">
-        <v>1</v>
+        <v>271</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="B145" s="1" t="n">
-        <v>2</v>
+        <v>272</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="B146" s="1" t="n">
-        <v>3</v>
+        <v>273</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="B147" s="1" t="n">
-        <v>4</v>
+        <v>274</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="B148" s="1" t="n">
-        <v>5</v>
+        <v>275</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B149" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B150" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B151" s="1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="B152" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>276</v>
+        <v>280</v>
+      </c>
+      <c r="B153" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
+      </c>
+      <c r="B154" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
+      </c>
+      <c r="B155" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
+      </c>
+      <c r="B156" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="B157" s="1" t="s">
         <v>284</v>
+      </c>
+      <c r="B157" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="B158" s="1" t="s">
-        <v>286</v>
+      <c r="B158" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B163" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="B164" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B168" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B169" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B169" s="1" t="s">
+    </row>
+    <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="0" t="s">
+      <c r="B170" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="B170" s="0" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>311</v>
@@ -2606,11 +2639,11 @@
         <v>319</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B176" s="0" t="s">
         <v>321</v>
       </c>
     </row>
@@ -2619,31 +2652,31 @@
         <v>322</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B178" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B179" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B180" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2691,31 +2724,79 @@
         <v>339</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B187" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="B188" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="B189" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B189" s="1" t="s">
+    </row>
+    <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
         <v>346</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add UUIDs. Start work on Nexus. Minor updates to Monolith and Fracture1. Fix some issues with ParticleEmitters.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="360">
   <si>
     <t>en</t>
   </si>
@@ -59,10 +59,16 @@
     <t>6 | Fracture</t>
   </si>
   <si>
+    <t>map nexus</t>
+  </si>
+  <si>
+    <t>7 | Nexus</t>
+  </si>
+  <si>
     <t>map valley</t>
   </si>
   <si>
-    <t>7 | Valley</t>
+    <t>8 | Valley</t>
   </si>
   <si>
     <t>toggle fullscreen tooltip</t>
@@ -1224,10 +1230,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1307,7 +1313,7 @@
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1315,7 +1321,7 @@
       <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1452,15 +1458,15 @@
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,19 +1781,19 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1927,19 +1933,19 @@
         <v>170</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="4" t="s">
         <v>174</v>
       </c>
     </row>
@@ -1967,7 +1973,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>181</v>
       </c>
@@ -1975,7 +1981,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>183</v>
       </c>
@@ -1996,12 +2002,12 @@
         <v>187</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>189</v>
@@ -2148,23 +2154,23 @@
         <v>224</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>31</v>
+        <v>226</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>31</v>
+        <v>226</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>225</v>
+        <v>33</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>226</v>
+        <v>33</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,11 +2229,11 @@
         <v>240</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="B124" s="0" t="s">
+      <c r="B124" s="1" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2271,33 +2277,33 @@
         <v>252</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>253</v>
+      <c r="B130" s="0" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>257</v>
@@ -2308,28 +2314,28 @@
         <v>258</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>262</v>
@@ -2356,159 +2362,159 @@
         <v>267</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="B149" s="1" t="n">
-        <v>0</v>
+        <v>277</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B150" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B151" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B152" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B153" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B154" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B155" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B156" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B157" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="B159" s="1" t="s">
         <v>287</v>
+      </c>
+      <c r="B159" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2639,25 +2645,25 @@
         <v>319</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="B176" s="0" t="s">
+      <c r="B176" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="B177" s="1" t="s">
-        <v>322</v>
+      <c r="B177" s="0" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>324</v>
@@ -2724,15 +2730,15 @@
         <v>339</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2799,8 +2805,16 @@
         <v>357</v>
       </c>
     </row>
+    <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048576">
+  <conditionalFormatting sqref="C2:C1048575">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
VR UI is looking pretty good, just a few things left.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="362">
   <si>
     <t>en</t>
   </si>
@@ -414,6 +414,12 @@
   </si>
   <si>
     <t>Toggle fullscreen</t>
+  </si>
+  <si>
+    <t>recenter pose</t>
+  </si>
+  <si>
+    <t>Recenter VR pose</t>
   </si>
   <si>
     <t>new game</t>
@@ -1230,10 +1236,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1789,19 +1795,19 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="4" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1941,19 +1947,19 @@
         <v>172</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="4" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1981,7 +1987,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>183</v>
       </c>
@@ -1989,7 +1995,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>185</v>
       </c>
@@ -2010,12 +2016,12 @@
         <v>189</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>191</v>
@@ -2162,23 +2168,23 @@
         <v>226</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>33</v>
+        <v>228</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>33</v>
+        <v>228</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>228</v>
+        <v>33</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2237,11 +2243,11 @@
         <v>242</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B125" s="0" t="s">
+      <c r="B125" s="1" t="s">
         <v>244</v>
       </c>
     </row>
@@ -2285,33 +2291,33 @@
         <v>254</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>255</v>
+      <c r="B131" s="0" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>259</v>
@@ -2322,28 +2328,28 @@
         <v>260</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>264</v>
@@ -2370,159 +2376,159 @@
         <v>269</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="B150" s="1" t="n">
-        <v>0</v>
+        <v>279</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B151" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B152" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B153" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B154" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B155" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B156" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B157" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="B160" s="1" t="s">
         <v>289</v>
+      </c>
+      <c r="B160" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,25 +2659,25 @@
         <v>321</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="B177" s="0" t="s">
+      <c r="B177" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="B178" s="1" t="s">
-        <v>324</v>
+      <c r="B178" s="0" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>326</v>
@@ -2738,15 +2744,15 @@
         <v>341</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2813,8 +2819,16 @@
         <v>359</v>
       </c>
     </row>
+    <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048575">
+  <conditionalFormatting sqref="C2:C1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Config improvements. Water is less dense so the player floats lower in it. New swimming animations. Better camera placement. VR improvements.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="364">
   <si>
     <t>en</t>
   </si>
@@ -164,13 +164,13 @@
     <t>reset options?</t>
   </si>
   <si>
-    <t>Reset to factory defaults and exit the game?</t>
+    <t>Reset options and control bindings?</t>
   </si>
   <si>
     <t>reset</t>
   </si>
   <si>
-    <t>Reset and exit</t>
+    <t>Reset</t>
   </si>
   <si>
     <t>modify setting</t>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t>Recenter VR pose</t>
+  </si>
+  <si>
+    <t>recenter pose button</t>
+  </si>
+  <si>
+    <t>Recenter VR pose [{{RecenterVRPose}}]</t>
   </si>
   <si>
     <t>new game</t>
@@ -1236,10 +1242,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1803,19 +1809,19 @@
         <v>136</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="4" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1955,19 +1961,19 @@
         <v>174</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="4" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1995,7 +2001,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>185</v>
       </c>
@@ -2003,7 +2009,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>187</v>
       </c>
@@ -2024,12 +2030,12 @@
         <v>191</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>193</v>
@@ -2176,23 +2182,23 @@
         <v>228</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>33</v>
+        <v>230</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>33</v>
+        <v>230</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>229</v>
+        <v>33</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>230</v>
+        <v>33</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2251,11 +2257,11 @@
         <v>244</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="B126" s="0" t="s">
+      <c r="B126" s="1" t="s">
         <v>246</v>
       </c>
     </row>
@@ -2299,33 +2305,33 @@
         <v>256</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="B132" s="1" t="s">
-        <v>257</v>
+      <c r="B132" s="0" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>261</v>
@@ -2336,28 +2342,28 @@
         <v>262</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>266</v>
@@ -2384,159 +2390,159 @@
         <v>271</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="B151" s="1" t="n">
-        <v>0</v>
+        <v>281</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B152" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B153" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B154" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B155" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B156" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B157" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="B161" s="1" t="s">
         <v>291</v>
+      </c>
+      <c r="B161" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2667,25 +2673,25 @@
         <v>323</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="B178" s="0" t="s">
+      <c r="B178" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="B179" s="1" t="s">
-        <v>326</v>
+      <c r="B179" s="0" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>328</v>
@@ -2752,15 +2758,15 @@
         <v>343</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2825,6 +2831,14 @@
       </c>
       <c r="B197" s="1" t="s">
         <v>361</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retry button for challenge maps. Turrets no longer shoot you while you're swimming. Fix animation bug when wall-running out of water. Fix some bugs with the block prediction mechanic. Disable kicking in the water. Fix a scaling bug with the voxel editor visualizations.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="366">
   <si>
     <t>en</t>
   </si>
@@ -468,6 +468,12 @@
   </si>
   <si>
     <t>Load</t>
+  </si>
+  <si>
+    <t>retry</t>
+  </si>
+  <si>
+    <t>Retry</t>
   </si>
   <si>
     <t>demo</t>
@@ -1242,10 +1248,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1969,19 +1975,19 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="4" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2009,7 +2015,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>187</v>
       </c>
@@ -2017,7 +2023,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>189</v>
       </c>
@@ -2038,12 +2044,12 @@
         <v>193</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>195</v>
@@ -2190,23 +2196,23 @@
         <v>230</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>33</v>
+        <v>232</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>33</v>
+        <v>232</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>231</v>
+        <v>33</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>232</v>
+        <v>33</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2265,11 +2271,11 @@
         <v>246</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="B127" s="0" t="s">
+      <c r="B127" s="1" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2313,33 +2319,33 @@
         <v>258</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>259</v>
+      <c r="B133" s="0" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>263</v>
@@ -2350,28 +2356,28 @@
         <v>264</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>268</v>
@@ -2398,159 +2404,159 @@
         <v>273</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="B152" s="1" t="n">
-        <v>0</v>
+        <v>283</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B153" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B154" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B155" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B156" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B157" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="B162" s="1" t="s">
         <v>293</v>
+      </c>
+      <c r="B162" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2681,25 +2687,25 @@
         <v>325</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="B179" s="0" t="s">
+      <c r="B179" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="B180" s="1" t="s">
-        <v>328</v>
+      <c r="B180" s="0" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>330</v>
@@ -2766,15 +2772,15 @@
         <v>345</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2839,6 +2845,14 @@
       </c>
       <c r="B198" s="1" t="s">
         <v>363</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaks to the challenge level stuff in general. Fix a bug which prevented the player Die event from triggering sometimes.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="368">
   <si>
     <t>en</t>
   </si>
@@ -59,16 +59,16 @@
     <t>6 | Fracture</t>
   </si>
   <si>
+    <t>map valley</t>
+  </si>
+  <si>
+    <t>7 | Valley</t>
+  </si>
+  <si>
     <t>map nexus</t>
   </si>
   <si>
-    <t>7 | Nexus</t>
-  </si>
-  <si>
-    <t>map valley</t>
-  </si>
-  <si>
-    <t>8 | Valley</t>
+    <t>8 | Nexus</t>
   </si>
   <si>
     <t>toggle fullscreen tooltip</t>
@@ -437,7 +437,7 @@
     <t>alpha disclaimer</t>
   </si>
   <si>
-    <t>This is an ALPHA release. Animations and other assets are not final.</t>
+    <t>Disclaimer: this is an Alpha release. Assets are not final.</t>
   </si>
   <si>
     <t>play</t>
@@ -500,6 +500,12 @@
     <t>Switch to edit mode</t>
   </si>
   <si>
+    <t>level editor</t>
+  </si>
+  <si>
+    <t>Level editor</t>
+  </si>
+  <si>
     <t>credits</t>
   </si>
   <si>
@@ -515,7 +521,7 @@
     <t>challenge levels</t>
   </si>
   <si>
-    <t>Challenge Levels</t>
+    <t>Challenge levels</t>
   </si>
   <si>
     <t>challenge title</t>
@@ -527,13 +533,13 @@
     <t>official levels</t>
   </si>
   <si>
-    <t>Official Levels</t>
+    <t>Official levels</t>
   </si>
   <si>
     <t>workshop levels</t>
   </si>
   <si>
-    <t>Workshop Levels</t>
+    <t>Workshop levels</t>
   </si>
   <si>
     <t>downloading workshop maps</t>
@@ -1248,10 +1254,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1327,11 +1333,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="0" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1983,19 +1989,19 @@
         <v>178</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="4" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2023,7 +2029,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>189</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>191</v>
       </c>
@@ -2052,12 +2058,12 @@
         <v>195</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>197</v>
@@ -2204,23 +2210,23 @@
         <v>232</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>33</v>
+        <v>234</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>33</v>
+        <v>234</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>233</v>
+        <v>33</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>234</v>
+        <v>33</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2279,11 +2285,11 @@
         <v>248</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="B128" s="0" t="s">
+      <c r="B128" s="1" t="s">
         <v>250</v>
       </c>
     </row>
@@ -2327,33 +2333,33 @@
         <v>260</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>261</v>
+      <c r="B134" s="0" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>265</v>
@@ -2364,28 +2370,28 @@
         <v>266</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>270</v>
@@ -2412,159 +2418,159 @@
         <v>275</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="B153" s="1" t="n">
-        <v>0</v>
+        <v>285</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B154" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B155" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B156" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B157" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="B163" s="1" t="s">
         <v>295</v>
+      </c>
+      <c r="B163" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2695,25 +2701,25 @@
         <v>327</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="B180" s="0" t="s">
+      <c r="B180" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
         <v>330</v>
       </c>
-      <c r="B181" s="1" t="s">
-        <v>330</v>
+      <c r="B181" s="0" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>332</v>
@@ -2780,15 +2786,15 @@
         <v>347</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2853,6 +2859,14 @@
       </c>
       <c r="B199" s="1" t="s">
         <v>365</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvements to the Counter and VoxelSetter entities. Fix a propagation bug related to the HardPowered material. Fix several time trial issues. Tweak the slide. Fix text wrap on some menu items.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="374">
   <si>
     <t>en</t>
   </si>
@@ -458,6 +458,18 @@
     <t>Resume</t>
   </si>
   <si>
+    <t>save title</t>
+  </si>
+  <si>
+    <t>S A V E</t>
+  </si>
+  <si>
+    <t>load title</t>
+  </si>
+  <si>
+    <t>L O A D</t>
+  </si>
+  <si>
     <t>save</t>
   </si>
   <si>
@@ -528,6 +540,12 @@
   </si>
   <si>
     <t>C H A L L E N G E</t>
+  </si>
+  <si>
+    <t>challenge warning</t>
+  </si>
+  <si>
+    <t>Warning: some levels may require advanced techniques.</t>
   </si>
   <si>
     <t>official levels</t>
@@ -1254,10 +1272,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1973,7 +1991,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>175</v>
       </c>
@@ -1997,11 +2015,11 @@
         <v>180</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="1" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2021,11 +2039,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="4" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2037,7 +2055,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>191</v>
       </c>
@@ -2061,33 +2079,33 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>197</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>203</v>
@@ -2218,39 +2236,39 @@
         <v>234</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>33</v>
+        <v>236</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>33</v>
+        <v>237</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>239</v>
+        <v>33</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>240</v>
+        <v>33</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2293,27 +2311,27 @@
         <v>250</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="B129" s="0" t="s">
+      <c r="B129" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="B130" s="0" t="s">
+      <c r="B130" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="B131" s="0" t="s">
+      <c r="B131" s="1" t="s">
         <v>256</v>
       </c>
     </row>
@@ -2341,81 +2359,81 @@
         <v>262</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="0" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>265</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>276</v>
@@ -2426,175 +2444,175 @@
         <v>277</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="B154" s="1" t="n">
-        <v>0</v>
+        <v>289</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="B155" s="1" t="n">
-        <v>1</v>
+        <v>290</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="B156" s="1" t="n">
-        <v>2</v>
+        <v>291</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B157" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
+      </c>
+      <c r="B164" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
+      </c>
+      <c r="B165" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="B166" s="1" t="s">
         <v>301</v>
+      </c>
+      <c r="B166" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,11 +2727,11 @@
         <v>329</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
         <v>330</v>
       </c>
-      <c r="B181" s="0" t="s">
+      <c r="B181" s="1" t="s">
         <v>331</v>
       </c>
     </row>
@@ -2722,28 +2740,28 @@
         <v>332</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="B184" s="1" t="s">
         <v>336</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>338</v>
@@ -2794,31 +2812,31 @@
         <v>349</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2867,6 +2885,30 @@
       </c>
       <c r="B200" s="1" t="s">
         <v>367</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweak run animation speed. Add new lightramp. Hide editor UI while workshop interface is active. Rename some settings.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -248,10 +248,10 @@
     <t>Ambient occlusion</t>
   </si>
   <si>
-    <t>god rays</t>
-  </si>
-  <si>
-    <t>God rays</t>
+    <t>volumetric lighting</t>
+  </si>
+  <si>
+    <t>Volumetric lighting</t>
   </si>
   <si>
     <t>bloom</t>
@@ -1274,8 +1274,8 @@
   </sheetPr>
   <dimension ref="A1:C203"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Fix some minor localization crashes. Bump version number.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="376">
   <si>
     <t>en</t>
   </si>
@@ -438,6 +438,12 @@
   </si>
   <si>
     <t>Disclaimer: this is an Alpha release. Assets are not final.</t>
+  </si>
+  <si>
+    <t>build number</t>
+  </si>
+  <si>
+    <t>Build {0}</t>
   </si>
   <si>
     <t>play</t>
@@ -1272,10 +1278,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C203"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72:B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1991,7 +1997,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>175</v>
       </c>
@@ -1999,7 +2005,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>177</v>
       </c>
@@ -2039,19 +2045,19 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="4" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2079,7 +2085,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>197</v>
       </c>
@@ -2087,7 +2093,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>199</v>
       </c>
@@ -2108,12 +2114,12 @@
         <v>203</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>205</v>
@@ -2260,23 +2266,23 @@
         <v>240</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>33</v>
+        <v>242</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>33</v>
+        <v>242</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>241</v>
+        <v>33</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>242</v>
+        <v>33</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2335,11 +2341,11 @@
         <v>256</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="B132" s="0" t="s">
+      <c r="B132" s="1" t="s">
         <v>258</v>
       </c>
     </row>
@@ -2383,33 +2389,33 @@
         <v>268</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>269</v>
+      <c r="B138" s="0" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>273</v>
@@ -2420,28 +2426,28 @@
         <v>274</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>278</v>
@@ -2468,159 +2474,159 @@
         <v>283</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="B157" s="1" t="n">
-        <v>0</v>
+        <v>293</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B164" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B165" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B166" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="B167" s="1" t="s">
         <v>303</v>
+      </c>
+      <c r="B167" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2751,25 +2757,25 @@
         <v>335</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="B184" s="0" t="s">
+      <c r="B184" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="B185" s="1" t="s">
-        <v>338</v>
+      <c r="B185" s="0" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>340</v>
@@ -2836,15 +2842,15 @@
         <v>355</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,6 +2915,14 @@
       </c>
       <c r="B203" s="1" t="s">
         <v>373</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix some issues with VoxelAttachables. Update the map list. Add a key repeat delay after the first movement in voxel edit mode.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -65,10 +65,10 @@
     <t>7 | Valley</t>
   </si>
   <si>
-    <t>map nexus</t>
-  </si>
-  <si>
-    <t>8 | Nexus</t>
+    <t>map victims</t>
+  </si>
+  <si>
+    <t>8 | Victims</t>
   </si>
   <si>
     <t>toggle fullscreen tooltip</t>
@@ -1280,8 +1280,8 @@
   </sheetPr>
   <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72:B72"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Fix custom gamma setting. Update menu with new level structure. Demo mode is gone. Tweak voxel editor movement.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="374">
   <si>
     <t>en</t>
   </si>
@@ -23,52 +23,46 @@
     <t>ru</t>
   </si>
   <si>
-    <t>map apartment</t>
-  </si>
-  <si>
-    <t>1 | Apartment</t>
-  </si>
-  <si>
     <t>map rain</t>
   </si>
   <si>
-    <t>2 | Rain</t>
+    <t>1 | Rain</t>
   </si>
   <si>
     <t>map dawn</t>
   </si>
   <si>
-    <t>3 | Dawn</t>
+    <t>2 | Dawn</t>
   </si>
   <si>
     <t>map forest</t>
   </si>
   <si>
-    <t>4 | Forest</t>
+    <t>3 | Forest</t>
   </si>
   <si>
     <t>map monolith</t>
   </si>
   <si>
-    <t>5 | Monolith</t>
+    <t>4 | Monolith</t>
   </si>
   <si>
     <t>map fracture</t>
   </si>
   <si>
-    <t>6 | Fracture</t>
+    <t>5 | Fracture</t>
   </si>
   <si>
     <t>map valley</t>
   </si>
   <si>
-    <t>7 | Valley</t>
+    <t>6 | Valley</t>
   </si>
   <si>
     <t>map victims</t>
   </si>
   <si>
-    <t>8 | Victims</t>
+    <t>7 | Victims</t>
   </si>
   <si>
     <t>toggle fullscreen tooltip</t>
@@ -1278,10 +1272,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1349,19 +1343,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1369,7 +1363,7 @@
       <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1506,15 +1500,15 @@
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,19 +1839,19 @@
         <v>136</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="1" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1997,7 +1991,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>175</v>
       </c>
@@ -2005,7 +1999,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>177</v>
       </c>
@@ -2045,19 +2039,19 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="1" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2085,7 +2079,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>197</v>
       </c>
@@ -2093,7 +2087,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>199</v>
       </c>
@@ -2114,12 +2108,12 @@
         <v>203</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>205</v>
@@ -2266,23 +2260,23 @@
         <v>240</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>242</v>
+        <v>31</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>242</v>
+        <v>31</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>33</v>
+        <v>241</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>33</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,11 +2335,11 @@
         <v>256</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" s="0" t="s">
         <v>258</v>
       </c>
     </row>
@@ -2389,33 +2383,33 @@
         <v>268</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="B138" s="0" t="s">
-        <v>270</v>
+      <c r="B138" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>273</v>
@@ -2426,28 +2420,28 @@
         <v>274</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>278</v>
@@ -2474,159 +2468,159 @@
         <v>283</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
+      </c>
+      <c r="B157" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B164" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B165" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B166" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="B167" s="1" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2757,25 +2751,25 @@
         <v>335</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B184" s="0" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="B185" s="0" t="s">
-        <v>339</v>
+      <c r="B185" s="1" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>340</v>
@@ -2842,15 +2836,15 @@
         <v>355</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B195" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,16 +2911,8 @@
         <v>373</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="0" t="s">
-        <v>374</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048576">
+  <conditionalFormatting sqref="C2:C1048575">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Separate waterfall Wwise events. Add water splash volume parameter and improve splash-out detection. Pull in DialogueLink and DialogueTrigger from the game repo. Add sound to Levitators. MessageDisplayers are no longer suspendable. Campaign scripts are no longer available in the release-mode level editor. Other stuff.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -65,10 +65,12 @@
     <t>7 | Victims</t>
   </si>
   <si>
-    <t>toggle fullscreen tooltip</t>
-  </si>
-  <si>
-    <t>[{{ToggleFullscreen}}] - Toggle Fullscreen</t>
+    <t>vr message</t>
+  </si>
+  <si>
+    <t>Read and follow all warnings and instructions included with the Headset before use. Headset should be calibrated for each user. Not for use by children under 13. Stop use if you experience any discomfort or health reactions.
+More: oculus.com/warnings
+Get in a relaxed position and press [{{RecenterVRPose}}] to calibrate and dismiss this message.</t>
   </si>
   <si>
     <t>okay</t>
@@ -413,13 +415,13 @@
     <t>recenter pose</t>
   </si>
   <si>
-    <t>Recenter VR pose</t>
+    <t>Recalibrate HMD</t>
   </si>
   <si>
     <t>recenter pose button</t>
   </si>
   <si>
-    <t>Recenter VR pose [{{RecenterVRPose}}]</t>
+    <t>Recalibrate HMD [{{RecenterVRPose}}]</t>
   </si>
   <si>
     <t>new game</t>
@@ -1274,8 +1276,8 @@
   </sheetPr>
   <dimension ref="A1:C203"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B68" activeCellId="0" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1351,7 +1353,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="132.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Add photo support to the phone. Fix powered block footstep propagation. Other minor tweaks.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="376">
   <si>
     <t>en</t>
   </si>
@@ -691,6 +691,18 @@
     <t>No service</t>
   </si>
   <si>
+    <t>messages</t>
+  </si>
+  <si>
+    <t>Messages</t>
+  </si>
+  <si>
+    <t>photos</t>
+  </si>
+  <si>
+    <t>Photos</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
@@ -839,12 +851,6 @@
   </si>
   <si>
     <t>Capslock</t>
-  </si>
-  <si>
-    <t>Kana</t>
-  </si>
-  <si>
-    <t>Kanji</t>
   </si>
   <si>
     <t>Escape</t>
@@ -1276,8 +1282,8 @@
   </sheetPr>
   <dimension ref="A1:C203"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B68" activeCellId="0" sqref="B68"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2262,31 +2268,31 @@
         <v>240</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>31</v>
+        <v>242</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>31</v>
+        <v>243</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>243</v>
+        <v>31</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>244</v>
+        <v>31</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2337,19 +2343,19 @@
         <v>256</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="B132" s="0" t="s">
+      <c r="B132" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="B133" s="0" t="s">
+      <c r="B133" s="1" t="s">
         <v>260</v>
       </c>
     </row>
@@ -2385,161 +2391,161 @@
         <v>268</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B157" s="1" t="n">
         <v>0</v>
@@ -2547,7 +2553,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B158" s="1" t="n">
         <v>1</v>
@@ -2555,7 +2561,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B159" s="1" t="n">
         <v>2</v>
@@ -2563,7 +2569,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B160" s="1" t="n">
         <v>3</v>
@@ -2571,7 +2577,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B161" s="1" t="n">
         <v>4</v>
@@ -2579,7 +2585,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B162" s="1" t="n">
         <v>5</v>
@@ -2587,7 +2593,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B163" s="1" t="n">
         <v>6</v>
@@ -2595,7 +2601,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B164" s="1" t="n">
         <v>7</v>
@@ -2603,7 +2609,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B165" s="1" t="n">
         <v>8</v>
@@ -2611,7 +2617,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B166" s="1" t="n">
         <v>9</v>
@@ -2619,298 +2625,298 @@
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New sky assets. New RiftSpawner script. New Updater API. Remove "special ability" input binding. Rifts are a little less deadly now. Add FPS limit option. Camera shake is now a World property rather than a PlayerData property.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -154,13 +154,13 @@
     <t>reset options</t>
   </si>
   <si>
-    <t>Reset to factory defaults</t>
+    <t>Reset to defaults</t>
   </si>
   <si>
     <t>reset options?</t>
   </si>
   <si>
-    <t>Reset options and control bindings?</t>
+    <t>Reset to defaults?</t>
   </si>
   <si>
     <t>reset</t>
@@ -208,6 +208,12 @@
     <t>V-sync</t>
   </si>
   <si>
+    <t>fps limit</t>
+  </si>
+  <si>
+    <t>FPS limit</t>
+  </si>
+  <si>
     <t>gamma</t>
   </si>
   <si>
@@ -380,12 +386,6 @@
   </si>
   <si>
     <t>Roll / Kick</t>
-  </si>
-  <si>
-    <t>special ability</t>
-  </si>
-  <si>
-    <t>Special ability</t>
   </si>
   <si>
     <t>toggle phone</t>
@@ -1256,21 +1256,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -1282,8 +1267,8 @@
   </sheetPr>
   <dimension ref="A1:C203"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2920,11 +2905,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048575">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Levitators now stay away from exits and signal towers. Filter gamepad input on menu and phone UI. Decrease gamepad look sensitivity multiplier. Fix a bug where the phone answer menu could be pulled up on the photo screen. Fix a phone UI layout bug in VR. Disable phone photo screen when no photo is available. Remove "load_map" console command. Update template map to new data format.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -694,7 +694,7 @@
     <t>messages</t>
   </si>
   <si>
-    <t>Messages</t>
+    <t>SMS</t>
   </si>
   <si>
     <t>photos</t>
@@ -1267,8 +1267,8 @@
   </sheetPr>
   <dimension ref="A1:C203"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C:C"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B115" activeCellId="0" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Add "loading" notification. Speed up health regeneration.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="378">
   <si>
     <t>en</t>
   </si>
@@ -626,6 +626,12 @@
   </si>
   <si>
     <t>Saved</t>
+  </si>
+  <si>
+    <t>loading</t>
+  </si>
+  <si>
+    <t>Loading...</t>
   </si>
   <si>
     <t>...</t>
@@ -1265,10 +1271,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C203"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B115" activeCellId="0" sqref="B115"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A104" activeCellId="0" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2101,12 +2107,12 @@
         <v>203</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>205</v>
@@ -2269,23 +2275,23 @@
         <v>244</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>31</v>
+        <v>246</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>31</v>
+        <v>246</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>245</v>
+        <v>31</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>246</v>
+        <v>31</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,11 +2350,11 @@
         <v>260</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="B134" s="0" t="s">
+      <c r="B134" s="1" t="s">
         <v>262</v>
       </c>
     </row>
@@ -2392,33 +2398,33 @@
         <v>272</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="B140" s="1" t="s">
-        <v>273</v>
+      <c r="B140" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>277</v>
@@ -2429,12 +2435,12 @@
         <v>278</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>280</v>
@@ -2461,159 +2467,159 @@
         <v>285</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="B157" s="1" t="n">
-        <v>0</v>
+        <v>295</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B164" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B165" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B166" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="B167" s="1" t="s">
         <v>305</v>
+      </c>
+      <c r="B167" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2744,25 +2750,25 @@
         <v>337</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="B184" s="0" t="s">
+      <c r="B184" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="B185" s="1" t="s">
-        <v>340</v>
+      <c r="B185" s="0" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>342</v>
@@ -2829,15 +2835,15 @@
         <v>357</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2902,6 +2908,14 @@
       </c>
       <c r="B203" s="1" t="s">
         <v>375</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix a wall-run crash. Tone down the rift spawner a bit. "Notes" -> "unread notes"
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -652,13 +652,13 @@
     <t>one note</t>
   </si>
   <si>
-    <t>1 note</t>
+    <t>1 unread note</t>
   </si>
   <si>
     <t>note count</t>
   </si>
   <si>
-    <t>{0} notes</t>
+    <t>{0} unread notes</t>
   </si>
   <si>
     <t>notes read</t>
@@ -1273,8 +1273,8 @@
   </sheetPr>
   <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A104" activeCellId="0" sqref="A104"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B109" activeCellId="0" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Update Steamworks. Allow water reflection to be disabled individually. New UI sounds. Fix an issue with binding gamepad inputs. Fix a missing UI localization string.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="380">
   <si>
     <t>en</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>Reset</t>
+  </si>
+  <si>
+    <t>reset gamepad</t>
+  </si>
+  <si>
+    <t>[A] Reset</t>
   </si>
   <si>
     <t>modify setting</t>
@@ -1271,10 +1277,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B109" activeCellId="0" sqref="B109"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1499,15 +1505,15 @@
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,19 +1844,19 @@
         <v>136</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="4" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1990,7 +1996,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>175</v>
       </c>
@@ -1998,7 +2004,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>177</v>
       </c>
@@ -2038,19 +2044,19 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="4" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2078,7 +2084,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>197</v>
       </c>
@@ -2086,7 +2092,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>199</v>
       </c>
@@ -2115,12 +2121,12 @@
         <v>205</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>207</v>
@@ -2283,23 +2289,23 @@
         <v>246</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>31</v>
+        <v>248</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>247</v>
+        <v>31</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>248</v>
+        <v>31</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,11 +2364,11 @@
         <v>262</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="B135" s="0" t="s">
+      <c r="B135" s="1" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2406,33 +2412,33 @@
         <v>274</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>275</v>
+      <c r="B141" s="0" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>279</v>
@@ -2443,12 +2449,12 @@
         <v>280</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>282</v>
@@ -2475,159 +2481,159 @@
         <v>287</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="B158" s="1" t="n">
-        <v>0</v>
+        <v>297</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B164" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B165" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B166" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B167" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="B168" s="1" t="s">
         <v>307</v>
+      </c>
+      <c r="B168" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2758,25 +2764,25 @@
         <v>339</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="B185" s="0" t="s">
+      <c r="B185" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
         <v>342</v>
       </c>
-      <c r="B186" s="1" t="s">
-        <v>342</v>
+      <c r="B186" s="0" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>344</v>
@@ -2843,15 +2849,15 @@
         <v>359</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2916,6 +2922,14 @@
       </c>
       <c r="B204" s="1" t="s">
         <v>377</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvements to the input binding system, and how settings are saved. The console is now hidden behind a mystical cheat code.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -406,12 +406,6 @@
     <t>Quicksave</t>
   </si>
   <si>
-    <t>toggle console</t>
-  </si>
-  <si>
-    <t>Toggle console</t>
-  </si>
-  <si>
     <t>toggle fullscreen</t>
   </si>
   <si>
@@ -719,6 +713,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>god mode</t>
+  </si>
+  <si>
+    <t>GOD MODE ACTIVATED. Press [~] to toggle console.</t>
   </si>
   <si>
     <t>LeftMouseButton</t>
@@ -1279,8 +1279,8 @@
   </sheetPr>
   <dimension ref="A1:C205"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A101" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1844,19 +1844,19 @@
         <v>136</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="1" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1996,7 +1996,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>175</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>177</v>
       </c>
@@ -2044,19 +2044,19 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="1" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>197</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>199</v>
       </c>
@@ -2121,12 +2121,12 @@
         <v>205</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>207</v>
@@ -2228,7 +2228,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>232</v>
       </c>

</xml_diff>

<commit_message>
Fix shadow glitches. Fix a crash when rendering spot lights on low graphics setting.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -59,10 +59,10 @@
     <t>6 | Valley</t>
   </si>
   <si>
-    <t>map victims</t>
-  </si>
-  <si>
-    <t>7 | Victims</t>
+    <t>map mark</t>
+  </si>
+  <si>
+    <t>7 | Mark</t>
   </si>
   <si>
     <t>vr message</t>
@@ -1279,8 +1279,8 @@
   </sheetPr>
   <dimension ref="A1:C205"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A101" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Orbs work like notes now. Fix a LogicGate crash.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="378">
   <si>
     <t>en</t>
   </si>
@@ -679,16 +679,10 @@
     <t>{0} orbs</t>
   </si>
   <si>
-    <t>one orb collected</t>
-  </si>
-  <si>
-    <t>1 orb collected</t>
-  </si>
-  <si>
     <t>orbs collected</t>
   </si>
   <si>
-    <t>{0} orbs collected</t>
+    <t>{0} / {1} orbs collected</t>
   </si>
   <si>
     <t>no service</t>
@@ -1277,10 +1271,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C205"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B113" activeCellId="0" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2220,7 +2214,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>230</v>
       </c>
@@ -2228,7 +2222,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>232</v>
       </c>
@@ -2289,23 +2283,23 @@
         <v>246</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>248</v>
+        <v>31</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>248</v>
+        <v>31</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>31</v>
+        <v>247</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>31</v>
+        <v>248</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,11 +2358,11 @@
         <v>262</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" s="0" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2412,33 +2406,33 @@
         <v>274</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="B141" s="0" t="s">
-        <v>276</v>
+      <c r="B141" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>279</v>
@@ -2449,12 +2443,12 @@
         <v>280</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>282</v>
@@ -2481,159 +2475,159 @@
         <v>287</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
+      </c>
+      <c r="B158" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B164" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B165" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B166" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B167" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B168" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="B168" s="1" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2764,25 +2758,25 @@
         <v>339</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B185" s="0" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
         <v>342</v>
       </c>
-      <c r="B186" s="0" t="s">
-        <v>343</v>
+      <c r="B186" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>344</v>
@@ -2849,15 +2843,15 @@
         <v>359</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2922,14 +2916,6 @@
       </c>
       <c r="B204" s="1" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="205" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hopefully fix a graphics crash. Fix a menu crash. Update credits. Fix glitchy message animations. Update tutorial prompts. Sound update.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="384">
   <si>
     <t>en</t>
   </si>
@@ -707,6 +707,24 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>signal tower prompt</t>
+  </si>
+  <si>
+    <t>[{{TogglePhone}}] to use signal tower.</t>
+  </si>
+  <si>
+    <t>phone done prompt</t>
+  </si>
+  <si>
+    <t>[{{TogglePhone}}] to dismiss phone.</t>
+  </si>
+  <si>
+    <t>note prompt</t>
+  </si>
+  <si>
+    <t>[{{TogglePhone}}] to read note.</t>
   </si>
   <si>
     <t>god mode</t>
@@ -1271,10 +1289,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B113" activeCellId="0" sqref="B113"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2214,7 +2232,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>230</v>
       </c>
@@ -2238,7 +2256,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>236</v>
       </c>
@@ -2283,39 +2301,39 @@
         <v>246</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>31</v>
+        <v>249</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>251</v>
+        <v>31</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>252</v>
+        <v>31</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,27 +2376,27 @@
         <v>262</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="B135" s="0" t="s">
+      <c r="B135" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="B136" s="0" t="s">
+      <c r="B136" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="B137" s="0" t="s">
+      <c r="B137" s="1" t="s">
         <v>268</v>
       </c>
     </row>
@@ -2406,65 +2424,65 @@
         <v>274</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B141" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>286</v>
@@ -2475,175 +2493,175 @@
         <v>287</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="B158" s="1" t="n">
-        <v>0</v>
+        <v>299</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="B159" s="1" t="n">
-        <v>1</v>
+        <v>300</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="B160" s="1" t="n">
-        <v>2</v>
+        <v>301</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B164" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B165" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B166" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B167" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
+      </c>
+      <c r="B168" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
+      </c>
+      <c r="B169" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="B170" s="1" t="s">
         <v>311</v>
+      </c>
+      <c r="B170" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2758,11 +2776,11 @@
         <v>339</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="B185" s="0" t="s">
+      <c r="B185" s="1" t="s">
         <v>341</v>
       </c>
     </row>
@@ -2771,28 +2789,28 @@
         <v>342</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="B188" s="1" t="s">
         <v>346</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>348</v>
@@ -2843,31 +2861,31 @@
         <v>359</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2916,6 +2934,30 @@
       </c>
       <c r="B204" s="1" t="s">
         <v>377</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload analytics in the background. Remove error and analytics forms.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="397">
   <si>
     <t>en</t>
   </si>
@@ -310,6 +310,15 @@
     <t>Ultra</t>
   </si>
   <si>
+    <t>analytics</t>
+  </si>
+  <si>
+    <t>Analytics</t>
+  </si>
+  <si>
+    <t>Ask</t>
+  </si>
+  <si>
     <t>sound effect volume</t>
   </si>
   <si>
@@ -614,6 +623,36 @@
   </si>
   <si>
     <t>Exiting will erase any unsaved progress. Are you sure?</t>
+  </si>
+  <si>
+    <t>enable analytics</t>
+  </si>
+  <si>
+    <t>Sure</t>
+  </si>
+  <si>
+    <t>enable analytics gamepad</t>
+  </si>
+  <si>
+    <t>[A] Sure</t>
+  </si>
+  <si>
+    <t>disable analytics</t>
+  </si>
+  <si>
+    <t>No thanks</t>
+  </si>
+  <si>
+    <t>disable analytics gamepad</t>
+  </si>
+  <si>
+    <t>[B] No thanks</t>
+  </si>
+  <si>
+    <t>analytics prompt</t>
+  </si>
+  <si>
+    <t>Upload anonymous crash reports and gameplay analytics?</t>
   </si>
   <si>
     <t>saving</t>
@@ -1289,10 +1328,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C216"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1709,814 +1748,814 @@
         <v>99</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>31</v>
+        <v>249</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>31</v>
+        <v>250</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B137" s="1" t="s">
+    </row>
+    <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
+      <c r="B140" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B138" s="0" t="s">
+    </row>
+    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
+      <c r="B141" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B139" s="0" t="s">
+    </row>
+    <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
+      <c r="B142" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B140" s="0" t="s">
+    </row>
+    <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
+      <c r="B143" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="B141" s="0" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="B142" s="0" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="B143" s="0" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B147" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B148" s="0" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
+      <c r="B149" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="B149" s="1" t="s">
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="s">
+      <c r="B150" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="B150" s="1" t="s">
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
+      <c r="B151" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="B151" s="1" t="s">
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="B152" s="1" t="s">
+      <c r="B152" s="0" t="s">
         <v>293</v>
       </c>
     </row>
@@ -2549,415 +2588,487 @@
         <v>297</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="B161" s="1" t="n">
-        <v>0</v>
+        <v>306</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B162" s="1" t="n">
-        <v>1</v>
+        <v>307</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="B163" s="1" t="n">
-        <v>2</v>
+        <v>308</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="B164" s="1" t="n">
-        <v>3</v>
+        <v>309</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="B165" s="1" t="n">
-        <v>4</v>
+        <v>310</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="B166" s="1" t="n">
-        <v>5</v>
+        <v>311</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="B167" s="1" t="n">
-        <v>6</v>
+        <v>312</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="B168" s="1" t="n">
-        <v>7</v>
+        <v>313</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="B169" s="1" t="n">
-        <v>8</v>
+        <v>314</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B170" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>313</v>
+        <v>316</v>
+      </c>
+      <c r="B171" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
+      </c>
+      <c r="B172" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
+      </c>
+      <c r="B173" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="B174" s="1" t="s">
         <v>319</v>
+      </c>
+      <c r="B174" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="B175" s="1" t="s">
-        <v>321</v>
+      <c r="B175" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
+      </c>
+      <c r="B176" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
+      </c>
+      <c r="B177" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
+      </c>
+      <c r="B178" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
+      </c>
+      <c r="B179" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="B188" s="0" t="s">
-        <v>347</v>
+        <v>341</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>364</v>
+        <v>359</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="B207" s="1" t="s">
+    </row>
+    <row r="210" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
         <v>383</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New time trial UI with gamepad support.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="401">
   <si>
     <t>en</t>
   </si>
@@ -493,6 +493,12 @@
     <t>Load</t>
   </si>
   <si>
+    <t>next level</t>
+  </si>
+  <si>
+    <t>Next level</t>
+  </si>
+  <si>
     <t>retry</t>
   </si>
   <si>
@@ -653,6 +659,12 @@
   </si>
   <si>
     <t>Upload anonymous crash reports and gameplay analytics?</t>
+  </si>
+  <si>
+    <t>best time</t>
+  </si>
+  <si>
+    <t>Best: {0}</t>
   </si>
   <si>
     <t>saving</t>
@@ -1328,10 +1340,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C216"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2079,7 +2091,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>178</v>
       </c>
@@ -2087,7 +2099,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>180</v>
       </c>
@@ -2127,19 +2139,19 @@
         <v>189</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="4" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2167,7 +2179,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>200</v>
       </c>
@@ -2175,7 +2187,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>202</v>
       </c>
@@ -2207,7 +2219,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>210</v>
       </c>
@@ -2215,7 +2227,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>212</v>
       </c>
@@ -2244,20 +2256,20 @@
         <v>218</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>222</v>
@@ -2367,7 +2379,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>249</v>
       </c>
@@ -2383,7 +2395,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>253</v>
       </c>
@@ -2436,31 +2448,31 @@
         <v>265</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>31</v>
+        <v>267</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>31</v>
+        <v>268</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>268</v>
+        <v>31</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>269</v>
+        <v>31</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2511,19 +2523,19 @@
         <v>281</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="B147" s="0" t="s">
+      <c r="B147" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="B148" s="0" t="s">
+      <c r="B148" s="1" t="s">
         <v>285</v>
       </c>
     </row>
@@ -2559,57 +2571,57 @@
         <v>293</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B153" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>303</v>
@@ -2628,167 +2640,167 @@
         <v>306</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="B170" s="1" t="n">
-        <v>0</v>
+        <v>317</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="B171" s="1" t="n">
-        <v>1</v>
+        <v>318</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B172" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B173" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B174" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B175" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B176" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B177" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
+      </c>
+      <c r="B180" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="B181" s="1" t="s">
         <v>328</v>
+      </c>
+      <c r="B181" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2911,11 +2923,11 @@
         <v>358</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
         <v>359</v>
       </c>
-      <c r="B197" s="0" t="s">
+      <c r="B197" s="1" t="s">
         <v>360</v>
       </c>
     </row>
@@ -2924,20 +2936,20 @@
         <v>361</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="B199" s="1" t="s">
         <v>363</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>365</v>
@@ -2996,23 +3008,23 @@
         <v>378</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3069,6 +3081,22 @@
       </c>
       <c r="B216" s="1" t="s">
         <v>396</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove alpha disclaimer. Move cheat menu into new game menu and track which levels have been unlocked. New magic cube sounds. Better support for god mode. Fix a bug preventing spawning after exiting out of a cutscene.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="391">
   <si>
     <t>en</t>
   </si>
@@ -53,10 +53,10 @@
     <t>5 | Fracture</t>
   </si>
   <si>
-    <t>map valley</t>
-  </si>
-  <si>
-    <t>6 | Valley</t>
+    <t>map fortress</t>
+  </si>
+  <si>
+    <t>6 | Fortress</t>
   </si>
   <si>
     <t>map mark</t>
@@ -439,30 +439,12 @@
     <t>New game</t>
   </si>
   <si>
-    <t>alpha disclaimer</t>
-  </si>
-  <si>
-    <t>Disclaimer: this is an Alpha release. Assets are not final.</t>
-  </si>
-  <si>
     <t>build number</t>
   </si>
   <si>
     <t>Build {0}</t>
   </si>
   <si>
-    <t>play</t>
-  </si>
-  <si>
-    <t>Play</t>
-  </si>
-  <si>
-    <t>play gamepad</t>
-  </si>
-  <si>
-    <t>[A] Play</t>
-  </si>
-  <si>
     <t>resume</t>
   </si>
   <si>
@@ -505,22 +487,10 @@
     <t>Retry</t>
   </si>
   <si>
-    <t>demo</t>
-  </si>
-  <si>
-    <t>DEMO</t>
-  </si>
-  <si>
-    <t>cheat</t>
-  </si>
-  <si>
-    <t>Cheat</t>
-  </si>
-  <si>
-    <t>cheat title</t>
-  </si>
-  <si>
-    <t>C H E A T</t>
+    <t>start title</t>
+  </si>
+  <si>
+    <t>S T A R T</t>
   </si>
   <si>
     <t>edit mode</t>
@@ -1340,10 +1310,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C213"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B83" activeCellId="0" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1939,11 +1909,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="1" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2059,7 +2029,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>170</v>
       </c>
@@ -2099,7 +2069,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>180</v>
       </c>
@@ -2107,11 +2077,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="4" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2151,7 +2121,7 @@
       <c r="A100" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="1" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2227,49 +2197,49 @@
         <v>211</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>212</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>222</v>
@@ -2355,7 +2325,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>243</v>
       </c>
@@ -2395,7 +2365,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>253</v>
       </c>
@@ -2424,55 +2394,55 @@
         <v>259</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>261</v>
+        <v>31</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>262</v>
+        <v>31</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>31</v>
+        <v>268</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>31</v>
+        <v>269</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,43 +2469,43 @@
         <v>275</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" s="0" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" s="0" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B146" s="0" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" s="0" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" s="0" t="s">
         <v>285</v>
       </c>
     </row>
@@ -2547,260 +2517,260 @@
         <v>287</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B150" s="0" t="s">
+      <c r="B150" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
+      <c r="B151" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="B151" s="0" t="s">
+      <c r="B152" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
+      <c r="B153" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B152" s="0" t="s">
+    </row>
+    <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="B153" s="0" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="B154" s="0" t="s">
-        <v>297</v>
+      <c r="B154" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
+      </c>
+      <c r="B167" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
+      </c>
+      <c r="B168" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
+      </c>
+      <c r="B169" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
+      </c>
+      <c r="B170" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
+      </c>
+      <c r="B171" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B172" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B173" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B174" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B175" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B176" s="1" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="B177" s="1" t="n">
-        <v>5</v>
+        <v>319</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="B178" s="1" t="n">
-        <v>6</v>
+        <v>321</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="B179" s="1" t="n">
-        <v>7</v>
+        <v>323</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="B180" s="1" t="n">
-        <v>8</v>
+        <v>325</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="B181" s="1" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2899,11 +2869,11 @@
         <v>352</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="B194" s="1" t="s">
+      <c r="B194" s="0" t="s">
         <v>354</v>
       </c>
     </row>
@@ -2912,44 +2882,44 @@
         <v>355</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B197" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B198" s="1" t="s">
+    </row>
+    <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="0" t="s">
+      <c r="B199" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="B199" s="0" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>365</v>
@@ -2984,47 +2954,47 @@
         <v>372</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B205" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="B208" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3057,46 +3027,6 @@
       </c>
       <c r="B213" s="1" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="214" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="217" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="218" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="0" t="s">
-        <v>399</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New level editor achievement. Reverb zones. Fix predictive block visualization artifacts. Predictive blocks now match the color of magic cubes you're carrying. Big sound update. Fix a weird crash related to particle rendering. Steam leaderboards now show friends as well as global rank. Fix an issue with footstep events triggering every frame.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="399">
   <si>
     <t>en</t>
   </si>
@@ -655,6 +655,12 @@
     <t>Loading...</t>
   </si>
   <si>
+    <t>friends</t>
+  </si>
+  <si>
+    <t>Friends</t>
+  </si>
+  <si>
     <t>leaderboard</t>
   </si>
   <si>
@@ -740,6 +746,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>signal tower prompt</t>
@@ -1322,10 +1334,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C215"/>
+  <dimension ref="A1:C217"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A111" activeCellId="0" sqref="A111"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B127" activeCellId="0" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2230,12 +2242,12 @@
         <v>216</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>218</v>
@@ -2353,7 +2365,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>247</v>
       </c>
@@ -2369,7 +2381,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>251</v>
       </c>
@@ -2422,31 +2434,31 @@
         <v>263</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>31</v>
+        <v>265</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>31</v>
+        <v>266</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>266</v>
+        <v>31</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>267</v>
+        <v>31</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2497,19 +2509,19 @@
         <v>279</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="B146" s="0" t="s">
+      <c r="B146" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="B147" s="0" t="s">
+      <c r="B147" s="1" t="s">
         <v>283</v>
       </c>
     </row>
@@ -2545,57 +2557,57 @@
         <v>291</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>301</v>
@@ -2614,167 +2626,167 @@
         <v>304</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="B169" s="1" t="n">
-        <v>0</v>
+        <v>315</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="B170" s="1" t="n">
-        <v>1</v>
+        <v>316</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B171" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B172" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B173" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B174" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B175" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B176" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B177" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
+      </c>
+      <c r="B179" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="B180" s="1" t="s">
         <v>326</v>
+      </c>
+      <c r="B180" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2897,11 +2909,11 @@
         <v>356</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="B196" s="0" t="s">
+      <c r="B196" s="1" t="s">
         <v>358</v>
       </c>
     </row>
@@ -2910,20 +2922,20 @@
         <v>359</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="B198" s="1" t="s">
         <v>361</v>
+      </c>
+      <c r="B198" s="0" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>363</v>
@@ -2982,23 +2994,23 @@
         <v>376</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3055,6 +3067,22 @@
       </c>
       <c r="B215" s="1" t="s">
         <v>394</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sound update. Fix audio not pausing on alt-tab. Credits update.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="401">
   <si>
     <t>en</t>
   </si>
@@ -770,6 +770,12 @@
   </si>
   <si>
     <t>[{{TogglePhone}}] to read note.</t>
+  </si>
+  <si>
+    <t>endings</t>
+  </si>
+  <si>
+    <t>Of four possible endings, you chose ending “{0}”.</t>
   </si>
   <si>
     <t>god mode</t>
@@ -1334,10 +1340,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C217"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B127" activeCellId="0" sqref="B127"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A108" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B131" activeCellId="0" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2381,7 +2387,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>251</v>
       </c>
@@ -2389,7 +2395,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>253</v>
       </c>
@@ -2450,23 +2456,23 @@
         <v>267</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>31</v>
+        <v>269</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>31</v>
+        <v>269</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>268</v>
+        <v>31</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>269</v>
+        <v>31</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,11 +2531,11 @@
         <v>283</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="B148" s="0" t="s">
+      <c r="B148" s="1" t="s">
         <v>285</v>
       </c>
     </row>
@@ -2573,33 +2579,33 @@
         <v>295</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="B154" s="1" t="s">
-        <v>296</v>
+      <c r="B154" s="0" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>300</v>
@@ -2610,12 +2616,12 @@
         <v>301</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>303</v>
@@ -2642,159 +2648,159 @@
         <v>308</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="B171" s="1" t="n">
-        <v>0</v>
+        <v>318</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B172" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B173" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B174" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B175" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B176" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B177" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B180" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="B181" s="1" t="s">
         <v>328</v>
+      </c>
+      <c r="B181" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2925,25 +2931,25 @@
         <v>360</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
         <v>361</v>
       </c>
-      <c r="B198" s="0" t="s">
+      <c r="B198" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="B199" s="1" t="s">
-        <v>363</v>
+      <c r="B199" s="0" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>365</v>
@@ -3010,15 +3016,15 @@
         <v>380</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,6 +3089,14 @@
       </c>
       <c r="B217" s="1" t="s">
         <v>398</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix ambient sound bug. Audio update. Remove ice material. Add controller vibration option. Fix editor dropdown annoyances. Fix time trial crash when physics entities are active. Patch a huge fall damage exploit.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="403">
   <si>
     <t>en</t>
   </si>
@@ -353,6 +353,12 @@
   </si>
   <si>
     <t>Invert look Y</t>
+  </si>
+  <si>
+    <t>controller vibration</t>
+  </si>
+  <si>
+    <t>Controller vibration</t>
   </si>
   <si>
     <t>look sensitivity</t>
@@ -1340,10 +1346,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C219"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A108" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B131" activeCellId="0" sqref="B131"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2059,7 +2065,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>170</v>
       </c>
@@ -2067,7 +2073,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>172</v>
       </c>
@@ -2107,19 +2113,19 @@
         <v>181</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="4" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2147,7 +2153,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>192</v>
       </c>
@@ -2155,7 +2161,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>194</v>
       </c>
@@ -2187,7 +2193,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>202</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>204</v>
       </c>
@@ -2256,12 +2262,12 @@
         <v>218</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>220</v>
@@ -2395,7 +2401,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>253</v>
       </c>
@@ -2403,7 +2409,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>255</v>
       </c>
@@ -2464,23 +2470,23 @@
         <v>269</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>31</v>
+        <v>271</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>31</v>
+        <v>271</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>270</v>
+        <v>31</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>271</v>
+        <v>31</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,11 +2545,11 @@
         <v>285</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="B149" s="0" t="s">
+      <c r="B149" s="1" t="s">
         <v>287</v>
       </c>
     </row>
@@ -2587,33 +2593,33 @@
         <v>297</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>298</v>
       </c>
-      <c r="B155" s="1" t="s">
-        <v>298</v>
+      <c r="B155" s="0" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>302</v>
@@ -2624,12 +2630,12 @@
         <v>303</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>305</v>
@@ -2656,159 +2662,159 @@
         <v>310</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="B172" s="1" t="n">
-        <v>0</v>
+        <v>320</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B173" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B174" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B175" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B176" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B177" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B180" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B181" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="B182" s="1" t="s">
         <v>330</v>
+      </c>
+      <c r="B182" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2939,25 +2945,25 @@
         <v>362</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="B199" s="0" t="s">
+      <c r="B199" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="B200" s="1" t="s">
-        <v>365</v>
+      <c r="B200" s="0" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>367</v>
@@ -3024,15 +3030,15 @@
         <v>382</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3097,6 +3103,14 @@
       </c>
       <c r="B218" s="1" t="s">
         <v>400</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "get more" button to time trial UI. Fix missing menu localization key. Fix UI rendering in high-resolution screenshots.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="405">
   <si>
     <t>en</t>
   </si>
@@ -527,6 +527,12 @@
   </si>
   <si>
     <t>Challenge levels</t>
+  </si>
+  <si>
+    <t>get more</t>
+  </si>
+  <si>
+    <t>Get more</t>
   </si>
   <si>
     <t>challenge title</t>
@@ -1346,10 +1352,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C219"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2073,7 +2079,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>172</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>174</v>
       </c>
@@ -2121,19 +2127,19 @@
         <v>183</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="4" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2161,7 +2167,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>194</v>
       </c>
@@ -2169,7 +2175,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>196</v>
       </c>
@@ -2201,7 +2207,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>204</v>
       </c>
@@ -2209,7 +2215,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>206</v>
       </c>
@@ -2270,12 +2276,12 @@
         <v>220</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>222</v>
@@ -2409,7 +2415,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>255</v>
       </c>
@@ -2417,7 +2423,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>257</v>
       </c>
@@ -2478,23 +2484,23 @@
         <v>271</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>31</v>
+        <v>273</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>31</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>272</v>
+        <v>31</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>273</v>
+        <v>31</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2553,11 +2559,11 @@
         <v>287</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B150" s="0" t="s">
+      <c r="B150" s="1" t="s">
         <v>289</v>
       </c>
     </row>
@@ -2601,33 +2607,33 @@
         <v>299</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="B156" s="1" t="s">
-        <v>300</v>
+      <c r="B156" s="0" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>304</v>
@@ -2638,12 +2644,12 @@
         <v>305</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>307</v>
@@ -2670,159 +2676,159 @@
         <v>312</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="B173" s="1" t="n">
-        <v>0</v>
+        <v>322</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B174" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B175" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B176" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B177" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B180" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B181" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B182" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="B183" s="1" t="s">
         <v>332</v>
+      </c>
+      <c r="B183" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2953,25 +2959,25 @@
         <v>364</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="B200" s="0" t="s">
+      <c r="B200" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="B201" s="1" t="s">
-        <v>367</v>
+      <c r="B201" s="0" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>369</v>
@@ -3038,15 +3044,15 @@
         <v>384</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3111,6 +3117,14 @@
       </c>
       <c r="B219" s="1" t="s">
         <v>402</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sound update. Clean up unused console commands. Add option to disable waypoints. Fix spinner physics weirdness. Fix instant spawn bug after loading a save game. Fix voxel selection bug while dragging voxels. Fix load/save menu gamepad weirdness. Console can no longer be active unless the game is paused.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="407">
   <si>
     <t>en</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>Reticle</t>
+  </si>
+  <si>
+    <t>waypoints</t>
+  </si>
+  <si>
+    <t>Waypoints</t>
   </si>
   <si>
     <t>ambient occlusion</t>
@@ -1352,10 +1358,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1772,15 +1778,15 @@
         <v>99</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1793,10 +1799,10 @@
     </row>
     <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2087,7 +2093,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>174</v>
       </c>
@@ -2095,7 +2101,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>176</v>
       </c>
@@ -2135,19 +2141,19 @@
         <v>185</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="4" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2175,7 +2181,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>196</v>
       </c>
@@ -2183,7 +2189,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>198</v>
       </c>
@@ -2215,7 +2221,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>206</v>
       </c>
@@ -2223,7 +2229,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>208</v>
       </c>
@@ -2284,12 +2290,12 @@
         <v>222</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>224</v>
@@ -2423,7 +2429,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>257</v>
       </c>
@@ -2431,7 +2437,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>259</v>
       </c>
@@ -2492,23 +2498,23 @@
         <v>273</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>31</v>
+        <v>275</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>31</v>
+        <v>275</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>274</v>
+        <v>31</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>275</v>
+        <v>31</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2567,11 +2573,11 @@
         <v>289</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="B151" s="0" t="s">
+      <c r="B151" s="1" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2615,33 +2621,33 @@
         <v>301</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="B157" s="1" t="s">
-        <v>302</v>
+      <c r="B157" s="0" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>306</v>
@@ -2652,12 +2658,12 @@
         <v>307</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>309</v>
@@ -2684,159 +2690,159 @@
         <v>314</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="B174" s="1" t="n">
-        <v>0</v>
+        <v>324</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B175" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B176" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B177" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B180" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B181" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B182" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B183" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="B184" s="1" t="s">
         <v>334</v>
+      </c>
+      <c r="B184" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2967,25 +2973,25 @@
         <v>366</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="B201" s="0" t="s">
+      <c r="B201" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="B202" s="1" t="s">
-        <v>369</v>
+      <c r="B202" s="0" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>371</v>
@@ -3052,15 +3058,15 @@
         <v>386</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3125,6 +3131,14 @@
       </c>
       <c r="B220" s="1" t="s">
         <v>404</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweak analytics opt out prompt. Fix misleading error form message.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -619,34 +619,34 @@
     <t>Exiting will erase any unsaved progress. Are you sure?</t>
   </si>
   <si>
+    <t>disable analytics</t>
+  </si>
+  <si>
+    <t>Opt out</t>
+  </si>
+  <si>
+    <t>disable analytics gamepad</t>
+  </si>
+  <si>
+    <t>[B] Opt out</t>
+  </si>
+  <si>
     <t>enable analytics</t>
   </si>
   <si>
-    <t>Sure</t>
+    <t>It's fine</t>
   </si>
   <si>
     <t>enable analytics gamepad</t>
   </si>
   <si>
-    <t>[A] Sure</t>
-  </si>
-  <si>
-    <t>disable analytics</t>
-  </si>
-  <si>
-    <t>No thanks</t>
-  </si>
-  <si>
-    <t>disable analytics gamepad</t>
-  </si>
-  <si>
-    <t>[B] No thanks</t>
+    <t>[A] It's fine</t>
   </si>
   <si>
     <t>analytics prompt</t>
   </si>
   <si>
-    <t>Upload anonymous crash reports and gameplay analytics?</t>
+    <t>Opt out of anonymous crash reports and analytics?</t>
   </si>
   <si>
     <t>best time</t>
@@ -1360,8 +1360,8 @@
   </sheetPr>
   <dimension ref="A1:C221"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Add Polish translation. Update main menu version indicator / website / language selector. Bump version number.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="141"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="567">
   <si>
     <t>en</t>
   </si>
   <si>
-    <t>ru</t>
+    <t>pl</t>
   </si>
   <si>
     <t>map rain</t>
@@ -1238,16 +1237,495 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>1 | Deszcz</t>
+  </si>
+  <si>
+    <t>2 | Świt</t>
+  </si>
+  <si>
+    <t>3 | Las</t>
+  </si>
+  <si>
+    <t>4 | Monolit</t>
+  </si>
+  <si>
+    <t>5 | Odłamanie</t>
+  </si>
+  <si>
+    <t>6 | Twierdza</t>
+  </si>
+  <si>
+    <t>Anuluj</t>
+  </si>
+  <si>
+    <t>[B] Anuluj</t>
+  </si>
+  <si>
+    <t>Przesuń po więcej</t>
+  </si>
+  <si>
+    <t>[A] Akceptuj</t>
+  </si>
+  <si>
+    <t>Akceptuj</t>
+  </si>
+  <si>
+    <t>[{{QuickSave}}] by zrobić szybki zapis</t>
+  </si>
+  <si>
+    <t>Powrót</t>
+  </si>
+  <si>
+    <t>Zapisz jako nowy</t>
+  </si>
+  <si>
+    <t>Nadpisać ten zapis?</t>
+  </si>
+  <si>
+    <t>Nadpisz</t>
+  </si>
+  <si>
+    <t>[A] Nadpisz</t>
+  </si>
+  <si>
+    <t>Opcje</t>
+  </si>
+  <si>
+    <t>O P C J E</t>
+  </si>
+  <si>
+    <t>Przywróć domyślne</t>
+  </si>
+  <si>
+    <t>Przywrócić domyślne?</t>
+  </si>
+  <si>
+    <t>Resetuj</t>
+  </si>
+  <si>
+    <t>[A] Resetuj</t>
+  </si>
+  <si>
+    <t>[{{ToggleFullscreen}}] by przełączyć pełny ekran</t>
+  </si>
+  <si>
+    <t>Rozdzielczość</t>
+  </si>
+  <si>
+    <t>Pełny w oknie</t>
+  </si>
+  <si>
+    <t>Zapisz rozdzielczość</t>
+  </si>
+  <si>
+    <t>Uruchom pełny ekran [{{ToggleFullscreen}}]</t>
+  </si>
+  <si>
+    <t>Synch. Pionowa</t>
+  </si>
+  <si>
+    <t>Limit FPS</t>
+  </si>
+  <si>
+    <t>Pole widzenia</t>
+  </si>
+  <si>
+    <t>Rozmycie ruchu</t>
+  </si>
+  <si>
+    <t>Refleksy</t>
+  </si>
+  <si>
+    <t>Celownik</t>
+  </si>
+  <si>
+    <t>Znaczniki</t>
+  </si>
+  <si>
+    <t>Okluzja otoczenia</t>
+  </si>
+  <si>
+    <t>Oświetlenie wolumetryczne</t>
+  </si>
+  <si>
+    <t>Poświata</t>
+  </si>
+  <si>
+    <t>Wył.</t>
+  </si>
+  <si>
+    <t>Wł.</t>
+  </si>
+  <si>
+    <t>Cienie</t>
+  </si>
+  <si>
+    <t>Niskie</t>
+  </si>
+  <si>
+    <t>Średnie</t>
+  </si>
+  <si>
+    <t>Wysokie</t>
+  </si>
+  <si>
+    <t>Analityka</t>
+  </si>
+  <si>
+    <t>Zapytaj</t>
+  </si>
+  <si>
+    <t>Głośność dźwięków</t>
+  </si>
+  <si>
+    <t>Głośność muzyki</t>
+  </si>
+  <si>
+    <t>Sterowanie</t>
+  </si>
+  <si>
+    <t>S T E R O W A N I E</t>
+  </si>
+  <si>
+    <t>Odwróć oś X</t>
+  </si>
+  <si>
+    <t>Odwróć oś Y</t>
+  </si>
+  <si>
+    <t>Wibracje kontrolera</t>
+  </si>
+  <si>
+    <t>Czułość widzenia</t>
+  </si>
+  <si>
+    <t>Do przodu</t>
+  </si>
+  <si>
+    <t>W lewo</t>
+  </si>
+  <si>
+    <t>Do tyłu</t>
+  </si>
+  <si>
+    <t>W prawo</t>
+  </si>
+  <si>
+    <t>Skok</t>
+  </si>
+  <si>
+    <t>Obrót / Kopnięcie</t>
+  </si>
+  <si>
+    <t>Telefon</t>
+  </si>
+  <si>
+    <t>Szybki zapis</t>
+  </si>
+  <si>
+    <t>Przełącz pełny ekran</t>
+  </si>
+  <si>
+    <t>Skalibruj urządzenie VR</t>
+  </si>
+  <si>
+    <t>Skalibruj urządzenie VR [{{RecenterVRPose}}]</t>
+  </si>
+  <si>
+    <t>Nowa gra</t>
+  </si>
+  <si>
+    <t>Wersja {0}</t>
+  </si>
+  <si>
+    <t>Wznów</t>
+  </si>
+  <si>
+    <t>W C Z Y T A J</t>
+  </si>
+  <si>
+    <t>Z A P I S Z</t>
+  </si>
+  <si>
+    <t>Zapisz</t>
+  </si>
+  <si>
+    <t>Wczytaj</t>
+  </si>
+  <si>
+    <t>Następny poziom</t>
+  </si>
+  <si>
+    <t>Ponów</t>
+  </si>
+  <si>
+    <t>Przełącz do trybu edycji</t>
+  </si>
+  <si>
+    <t>Edytor poziomów</t>
+  </si>
+  <si>
+    <t>Autorzy</t>
+  </si>
+  <si>
+    <t>A U T O R Z Y</t>
+  </si>
+  <si>
+    <t>Wyzwania</t>
+  </si>
+  <si>
+    <t>Zdobądź więcej</t>
+  </si>
+  <si>
+    <t>W Y Z W A N I A</t>
+  </si>
+  <si>
+    <t>Uwaga: Niektóre etapy wymagają zaawansowanych technik.</t>
+  </si>
+  <si>
+    <t>Oficjalne etapy</t>
+  </si>
+  <si>
+    <t>Etapy z warsztatu Steam</t>
+  </si>
+  <si>
+    <t>Pobieranie {0} map z warsztatu…</t>
+  </si>
+  <si>
+    <t>Mapy zsynchronizowane!</t>
+  </si>
+  <si>
+    <t>Menu główne</t>
+  </si>
+  <si>
+    <t>Wyjdź do menu głównego</t>
+  </si>
+  <si>
+    <t>[A] Wyjdź do menu głównego</t>
+  </si>
+  <si>
+    <t>Wyjście</t>
+  </si>
+  <si>
+    <t>[A] Wyjście</t>
+  </si>
+  <si>
+    <t>Wyłącz analizę</t>
+  </si>
+  <si>
+    <t>[B] Wyłącz analizę</t>
+  </si>
+  <si>
+    <t>Jest w porządku</t>
+  </si>
+  <si>
+    <t>[A] Jest w porządku</t>
+  </si>
+  <si>
+    <t>Zrezygnować z anonimowych raportów i analiz w wypadku zawieszenia gry?</t>
+  </si>
+  <si>
+    <t>Najlepszy: {0}</t>
+  </si>
+  <si>
+    <t>Zapisywanie…</t>
+  </si>
+  <si>
+    <t>Zapisano</t>
+  </si>
+  <si>
+    <t>Ładowanie…</t>
+  </si>
+  <si>
+    <t>Znajomi</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Błąd synchronizacji rankingu.</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Napisz</t>
+  </si>
+  <si>
+    <t>[A] Napisz</t>
+  </si>
+  <si>
+    <t>1 nieprzeczytana notatka</t>
+  </si>
+  <si>
+    <t>{0} nieprzeczytane notatki</t>
+  </si>
+  <si>
+    <t>{0} / {1} przeczytanych notatek</t>
+  </si>
+  <si>
+    <t>1 nieodnaleziona sfera</t>
+  </si>
+  <si>
+    <t>{0} nieodnalezione sfery</t>
+  </si>
+  <si>
+    <t>{0} / {1} zdobytych sfer</t>
+  </si>
+  <si>
+    <t>Brak zasięgu</t>
+  </si>
+  <si>
+    <t>Zdjęcia</t>
+  </si>
+  <si>
+    <t>Tak</t>
+  </si>
+  <si>
+    <t>Nie</t>
+  </si>
+  <si>
+    <t>Z czterech możliwych zakończeń, wybrałeś zakończenie "{0}".</t>
+  </si>
+  <si>
+    <t>TRYB BOGA AKTYWOWANY. Naciśnij [~] by włączyć konsolę.</t>
+  </si>
+  <si>
+    <t>Lewy przycisk myszy</t>
+  </si>
+  <si>
+    <t>Środkowy przycisk myszy</t>
+  </si>
+  <si>
+    <t>Prawy przycisk myszy</t>
+  </si>
+  <si>
+    <t>Lewa łopatka</t>
+  </si>
+  <si>
+    <t>Prawa łopatka</t>
+  </si>
+  <si>
+    <t>Prawa zapadka</t>
+  </si>
+  <si>
+    <t>Lewa zapadka</t>
+  </si>
+  <si>
+    <t>Krzyżak - dół</t>
+  </si>
+  <si>
+    <t>Krzyżak - lewo</t>
+  </si>
+  <si>
+    <t>Krzyżak - prawo</t>
+  </si>
+  <si>
+    <t>Krzyżak - góra</t>
+  </si>
+  <si>
+    <t>Lewa gałka - przycisk</t>
+  </si>
+  <si>
+    <t>Prawa gałka - przycisk</t>
+  </si>
+  <si>
+    <t>Lewa gałka w lewo</t>
+  </si>
+  <si>
+    <t>Prawa gałka w górę</t>
+  </si>
+  <si>
+    <t>Prawa gałka w dół</t>
+  </si>
+  <si>
+    <t>Prawa gałka w prawo</t>
+  </si>
+  <si>
+    <t>Prawa gałka w lewo</t>
+  </si>
+  <si>
+    <t>Lewa gałka w górę</t>
+  </si>
+  <si>
+    <t>Lewa gałka w dół</t>
+  </si>
+  <si>
+    <t>Lewa gałka w prawo</t>
+  </si>
+  <si>
+    <t>Pauza</t>
+  </si>
+  <si>
+    <t>Esc</t>
+  </si>
+  <si>
+    <t>Spacja</t>
+  </si>
+  <si>
+    <t>Lewo</t>
+  </si>
+  <si>
+    <t>Góra</t>
+  </si>
+  <si>
+    <t>Prawo</t>
+  </si>
+  <si>
+    <t>Dół</t>
+  </si>
+  <si>
+    <t>Lewy klawisz windows</t>
+  </si>
+  <si>
+    <t>Prawy klawisz windows</t>
+  </si>
+  <si>
+    <t>Lewy shift</t>
+  </si>
+  <si>
+    <t>Prawy shift</t>
+  </si>
+  <si>
+    <t>Lewy control</t>
+  </si>
+  <si>
+    <t>Prawy control</t>
+  </si>
+  <si>
+    <t>Lewy alt</t>
+  </si>
+  <si>
+    <t>Prawy alt</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Przeczytaj wszystkie ostrzeżenia i instrukcje zawarte w zestawie przed jego użyciem. Okulary powinny być skalibrowane dla każdego użytkownika. Urządzenie nie jest wskazane dla dzieci poniżej 13 roku życia. Zakończ używanie jeżeli poczujesz dyskomfort lub mdłości.
+Więcej informacji: oculus.com/warnings
+Gdy będziesz w komfortowej pozycji, naciśnij [{{RecenterVRPose}}], by skalibrować urządzenie.</t>
+  </si>
+  <si>
+    <t>Zamknięcie spowoduje usunięcie niezapisanego postępu. Jesteś pewien?</t>
+  </si>
+  <si>
+    <t>[{{TogglePhone}}], by użyć przekaźnika.</t>
+  </si>
+  <si>
+    <t>[{{TogglePhone}}], by odrzucić telefon.</t>
+  </si>
+  <si>
+    <t>[{{TogglePhone}}], by przeczytać notatkę.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1255,22 +1733,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1286,7 +1749,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1294,86 +1757,335 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+  <a:themeElements>
+    <a:clrScheme name="Pakiet Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Pakiet Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Pakiet Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C221"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
+    <sheetView tabSelected="1" topLeftCell="B229" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.8775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="40.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.015306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="31.85546875"/>
+    <col min="2" max="2" width="40.85546875" style="1"/>
+    <col min="3" max="3" width="73.85546875" customWidth="1"/>
+    <col min="4" max="4" width="36.140625"/>
+    <col min="5" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1381,1771 +2093,2430 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="C2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="C3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="C4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="C5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="C6" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="C7" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="132.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="140.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="C9" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="C10" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="C11" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="C12" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="C13" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="C14" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="C15" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="C16" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="C17" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="C18" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="C19" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="C20" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="C21" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="C22" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="C23" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="C24" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="C25" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="C26" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="C27" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="C28" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
         <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="C29" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
         <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="C30" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
         <v>59</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="C31" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
         <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="C32" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
         <v>63</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="C33" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
         <v>65</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="C34" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
         <v>67</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>69</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="C36" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
         <v>71</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="C37" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
         <v>73</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="C38" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
         <v>75</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="C39" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
         <v>77</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="C40" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
         <v>79</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="C41" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
         <v>81</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="C42" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
         <v>83</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="C43" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
         <v>85</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="C44" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
         <v>87</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="C45" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
         <v>89</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="C46" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
         <v>91</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="C47" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
         <v>93</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="C48" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
         <v>95</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="C49" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
         <v>97</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="C50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
         <v>99</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="C51" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
         <v>101</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="C52" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
         <v>86</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="C53" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
         <v>88</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="C54" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
         <v>102</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="C55" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
         <v>104</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="C56" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
         <v>106</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="C57" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
         <v>108</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="C58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>110</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="C59" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
         <v>112</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="C60" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
         <v>114</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="C61" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
         <v>116</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="C62" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
         <v>118</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="C63" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
         <v>120</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="C64" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
         <v>122</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="C65" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
         <v>124</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="C66" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
         <v>126</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="C67" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
         <v>128</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="C68" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
         <v>130</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="C69" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
         <v>132</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="C70" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
         <v>134</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="C71" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
         <v>136</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="C72" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
         <v>138</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="C73" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
         <v>140</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="C74" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
         <v>142</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="C75" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
         <v>144</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="C76" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
         <v>146</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="C77" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
         <v>148</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="C78" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
         <v>150</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="C79" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
         <v>152</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="C80" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
         <v>154</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="C81" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
         <v>156</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="C82" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
         <v>158</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="C83" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
         <v>160</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="C84" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
         <v>162</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="C85" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
         <v>164</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="C86" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
         <v>166</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="C87" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
         <v>168</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="C88" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
         <v>170</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="C89" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
         <v>172</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="C90" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
         <v>174</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+      <c r="C91" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="25.5">
+      <c r="A92" t="s">
         <v>176</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="C92" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
         <v>178</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+      <c r="C93" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
         <v>180</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="C94" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
         <v>182</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="C95" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
         <v>184</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="C96" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
         <v>186</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="98" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="C97" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="25.5">
+      <c r="A98" t="s">
         <v>188</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="C98" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
         <v>190</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+      <c r="C99" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
         <v>192</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+      <c r="C100" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
         <v>194</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="C101" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
         <v>196</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+      <c r="C102" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="25.5">
+      <c r="A103" t="s">
         <v>198</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+      <c r="C103" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
         <v>200</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+      <c r="C104" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
         <v>202</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+      <c r="C105" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
         <v>204</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+      <c r="C106" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
         <v>206</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="108" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+      <c r="C107" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="25.5">
+      <c r="A108" t="s">
         <v>208</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="C108" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
         <v>210</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="C109" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
         <v>212</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="C110" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
         <v>214</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+      <c r="C111" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
         <v>216</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
+      <c r="C112" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
         <v>218</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+      <c r="C113" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
         <v>220</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+      <c r="C114" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
         <v>222</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+      <c r="C115" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
         <v>224</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="C116" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
         <v>225</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+      <c r="C117" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
         <v>227</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+      <c r="C118" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
         <v>229</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+      <c r="C119" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
         <v>231</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="C120" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
         <v>233</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="C121" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
         <v>235</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+      <c r="C122" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
         <v>237</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="C123" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
         <v>239</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+      <c r="C124" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
         <v>241</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
+      <c r="C125" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
         <v>243</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
+      <c r="C126" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
         <v>245</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
+      <c r="C127" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
         <v>247</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
+      <c r="C128" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
         <v>249</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+      <c r="C129" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
         <v>251</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
+      <c r="C130" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
         <v>253</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
+      <c r="C131" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
         <v>255</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
+      <c r="C132" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="25.5">
+      <c r="A133" t="s">
         <v>257</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="134" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
+      <c r="C133" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="25.5">
+      <c r="A134" t="s">
         <v>259</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
+      <c r="C134" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
         <v>261</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
+      <c r="C135" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
         <v>263</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
+      <c r="C136" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
         <v>265</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
+      <c r="C137" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
         <v>267</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
+      <c r="C138" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
         <v>269</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
+      <c r="C139" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
         <v>271</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
+      <c r="C140" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" t="s">
         <v>273</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
+      <c r="C141" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
         <v>275</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
+      <c r="C142" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
         <v>31</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
+      <c r="C143" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" t="s">
         <v>276</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
+      <c r="C144" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
         <v>278</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
+      <c r="C145" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
         <v>280</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
+      <c r="C146" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
         <v>282</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
+      <c r="C147" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
         <v>284</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
+      <c r="C148" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
         <v>286</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="s">
+      <c r="C149" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
         <v>288</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
+      <c r="C150" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" t="s">
         <v>290</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
+      <c r="C151" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
         <v>292</v>
       </c>
-      <c r="B152" s="0" t="s">
+      <c r="B152" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0" t="s">
+      <c r="C152" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
         <v>294</v>
       </c>
-      <c r="B153" s="0" t="s">
+      <c r="B153" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
+      <c r="C153" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" t="s">
         <v>296</v>
       </c>
-      <c r="B154" s="0" t="s">
+      <c r="B154" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="0" t="s">
+      <c r="C154" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="s">
         <v>298</v>
       </c>
-      <c r="B155" s="0" t="s">
+      <c r="B155" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="0" t="s">
+      <c r="C155" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
         <v>300</v>
       </c>
-      <c r="B156" s="0" t="s">
+      <c r="B156" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="0" t="s">
+      <c r="C156" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
         <v>302</v>
       </c>
-      <c r="B157" s="0" t="s">
+      <c r="B157" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="s">
+      <c r="C157" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
         <v>304</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="0" t="s">
+      <c r="C158" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
         <v>305</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
+      <c r="C159" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
         <v>306</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="s">
+      <c r="C160" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
         <v>307</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
+      <c r="C161" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
         <v>309</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
+      <c r="C162" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
         <v>310</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="s">
+      <c r="C163" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
         <v>312</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="0" t="s">
+      <c r="C164" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
         <v>314</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0" t="s">
+      <c r="C165" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
         <v>316</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="0" t="s">
+      <c r="C166" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" t="s">
         <v>317</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="0" t="s">
+      <c r="C167" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" t="s">
         <v>318</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="0" t="s">
+      <c r="C168" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" t="s">
         <v>319</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="0" t="s">
+      <c r="C169" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" t="s">
         <v>320</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="0" t="s">
+      <c r="C170" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
         <v>321</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="0" t="s">
+      <c r="C171" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
         <v>322</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="0" t="s">
+      <c r="C172" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
         <v>323</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="0" t="s">
+      <c r="C173" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" t="s">
         <v>324</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="0" t="s">
+      <c r="C174" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" t="s">
         <v>325</v>
       </c>
-      <c r="B175" s="1" t="n">
+      <c r="B175" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="0" t="s">
+      <c r="C175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" t="s">
         <v>326</v>
       </c>
-      <c r="B176" s="1" t="n">
+      <c r="B176" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="0" t="s">
+      <c r="C176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" t="s">
         <v>327</v>
       </c>
-      <c r="B177" s="1" t="n">
+      <c r="B177" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
+      <c r="C177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" t="s">
         <v>328</v>
       </c>
-      <c r="B178" s="1" t="n">
+      <c r="B178" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="s">
+      <c r="C178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" t="s">
         <v>329</v>
       </c>
-      <c r="B179" s="1" t="n">
+      <c r="B179" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
+      <c r="C179">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" t="s">
         <v>330</v>
       </c>
-      <c r="B180" s="1" t="n">
+      <c r="B180" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
+      <c r="C180">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" t="s">
         <v>331</v>
       </c>
-      <c r="B181" s="1" t="n">
+      <c r="B181" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
+      <c r="C181">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" t="s">
         <v>332</v>
       </c>
-      <c r="B182" s="1" t="n">
+      <c r="B182" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
+      <c r="C182">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" t="s">
         <v>333</v>
       </c>
-      <c r="B183" s="1" t="n">
+      <c r="B183" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
+      <c r="C183">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" t="s">
         <v>334</v>
       </c>
-      <c r="B184" s="1" t="n">
+      <c r="B184" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
+      <c r="C184">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" t="s">
         <v>335</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
+      <c r="C185" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" t="s">
         <v>337</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="s">
+      <c r="C186" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" t="s">
         <v>339</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
+      <c r="C187" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="s">
         <v>341</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="s">
+      <c r="C188" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" t="s">
         <v>343</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="0" t="s">
+      <c r="C189" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" t="s">
         <v>345</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="s">
+      <c r="C190" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" t="s">
         <v>347</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="0" t="s">
+      <c r="C191" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" t="s">
         <v>349</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0" t="s">
+      <c r="C192" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" t="s">
         <v>351</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="0" t="s">
+      <c r="C193" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" t="s">
         <v>353</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="0" t="s">
+      <c r="C194" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" t="s">
         <v>355</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="0" t="s">
+      <c r="C195" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" t="s">
         <v>357</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="0" t="s">
+      <c r="C196" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" t="s">
         <v>359</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="0" t="s">
+      <c r="C197" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" t="s">
         <v>361</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="0" t="s">
+      <c r="C198" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" t="s">
         <v>363</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="0" t="s">
+      <c r="C199" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" t="s">
         <v>365</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="201" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="0" t="s">
+      <c r="C200" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" t="s">
         <v>367</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="0" t="s">
+      <c r="C201" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" t="s">
         <v>369</v>
       </c>
-      <c r="B202" s="0" t="s">
+      <c r="B202" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="203" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="0" t="s">
+      <c r="C202" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" t="s">
         <v>371</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="204" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="0" t="s">
+      <c r="C203" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" t="s">
         <v>372</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="205" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="0" t="s">
+      <c r="C204" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" t="s">
         <v>374</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="206" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="0" t="s">
+      <c r="C205" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" t="s">
         <v>376</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="207" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="0" t="s">
+      <c r="C206" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" t="s">
         <v>378</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="208" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="0" t="s">
+      <c r="C207" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" t="s">
         <v>380</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="209" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="0" t="s">
+      <c r="C208" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" t="s">
         <v>382</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="210" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="0" t="s">
+      <c r="C209" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" t="s">
         <v>384</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="211" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="0" t="s">
+      <c r="C210" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" t="s">
         <v>386</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="212" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="0" t="s">
+      <c r="C211" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" t="s">
         <v>388</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="213" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="0" t="s">
+      <c r="C212" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" t="s">
         <v>389</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="214" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="0" t="s">
+      <c r="C213" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" t="s">
         <v>391</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="215" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="0" t="s">
+      <c r="C214" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" t="s">
         <v>393</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="216" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="0" t="s">
+      <c r="C215" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" t="s">
         <v>395</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="217" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="0" t="s">
+      <c r="C216" s="5" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" t="s">
         <v>397</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="218" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="0" t="s">
+      <c r="C217" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" t="s">
         <v>399</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="219" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="0" t="s">
+      <c r="C218" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" t="s">
         <v>401</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="220" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="0" t="s">
+      <c r="C219" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" t="s">
         <v>403</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="221" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="0" t="s">
+      <c r="C220" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" t="s">
         <v>405</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>406</v>
       </c>
+      <c r="C221" t="s">
+        <v>406</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Update Polish translation. Show uncollected notes and orbs on pause menu. Move main menu build indicator / language selector to top right corner. Remove "vault over" move.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -1398,9 +1398,6 @@
     <t>Wibracje kontrolera</t>
   </si>
   <si>
-    <t>Czułość widzenia</t>
-  </si>
-  <si>
     <t>Do przodu</t>
   </si>
   <si>
@@ -1719,6 +1716,9 @@
   </si>
   <si>
     <t>[{{TogglePhone}}], by przeczytać notatkę.</t>
+  </si>
+  <si>
+    <t>Czułość kamery</t>
   </si>
 </sst>
 </file>
@@ -2072,8 +2072,8 @@
   </sheetPr>
   <dimension ref="A1:C221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B229" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+    <sheetView tabSelected="1" topLeftCell="B220" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2178,7 +2178,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2761,7 +2761,7 @@
         <v>117</v>
       </c>
       <c r="C62" t="s">
-        <v>460</v>
+        <v>566</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2772,7 +2772,7 @@
         <v>119</v>
       </c>
       <c r="C63" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2783,7 +2783,7 @@
         <v>121</v>
       </c>
       <c r="C64" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2794,7 +2794,7 @@
         <v>123</v>
       </c>
       <c r="C65" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2805,7 +2805,7 @@
         <v>125</v>
       </c>
       <c r="C66" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2816,7 +2816,7 @@
         <v>127</v>
       </c>
       <c r="C67" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2838,7 +2838,7 @@
         <v>131</v>
       </c>
       <c r="C69" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2849,7 +2849,7 @@
         <v>133</v>
       </c>
       <c r="C70" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2860,7 +2860,7 @@
         <v>135</v>
       </c>
       <c r="C71" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2871,7 +2871,7 @@
         <v>137</v>
       </c>
       <c r="C72" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2882,7 +2882,7 @@
         <v>139</v>
       </c>
       <c r="C73" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2893,7 +2893,7 @@
         <v>141</v>
       </c>
       <c r="C74" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2904,7 +2904,7 @@
         <v>143</v>
       </c>
       <c r="C75" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2915,7 +2915,7 @@
         <v>145</v>
       </c>
       <c r="C76" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2926,7 +2926,7 @@
         <v>147</v>
       </c>
       <c r="C77" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2937,7 +2937,7 @@
         <v>149</v>
       </c>
       <c r="C78" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2948,7 +2948,7 @@
         <v>151</v>
       </c>
       <c r="C79" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2959,7 +2959,7 @@
         <v>153</v>
       </c>
       <c r="C80" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2970,7 +2970,7 @@
         <v>155</v>
       </c>
       <c r="C81" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2981,7 +2981,7 @@
         <v>157</v>
       </c>
       <c r="C82" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2992,7 +2992,7 @@
         <v>159</v>
       </c>
       <c r="C83" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -3014,7 +3014,7 @@
         <v>163</v>
       </c>
       <c r="C85" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -3025,7 +3025,7 @@
         <v>165</v>
       </c>
       <c r="C86" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -3036,7 +3036,7 @@
         <v>167</v>
       </c>
       <c r="C87" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -3047,7 +3047,7 @@
         <v>169</v>
       </c>
       <c r="C88" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -3058,7 +3058,7 @@
         <v>171</v>
       </c>
       <c r="C89" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -3069,7 +3069,7 @@
         <v>173</v>
       </c>
       <c r="C90" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -3080,7 +3080,7 @@
         <v>175</v>
       </c>
       <c r="C91" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="25.5">
@@ -3091,7 +3091,7 @@
         <v>177</v>
       </c>
       <c r="C92" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -3102,7 +3102,7 @@
         <v>179</v>
       </c>
       <c r="C93" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -3113,7 +3113,7 @@
         <v>181</v>
       </c>
       <c r="C94" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -3124,7 +3124,7 @@
         <v>183</v>
       </c>
       <c r="C95" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -3135,7 +3135,7 @@
         <v>185</v>
       </c>
       <c r="C96" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -3146,7 +3146,7 @@
         <v>187</v>
       </c>
       <c r="C97" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="25.5">
@@ -3157,7 +3157,7 @@
         <v>189</v>
       </c>
       <c r="C98" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -3168,7 +3168,7 @@
         <v>191</v>
       </c>
       <c r="C99" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -3179,7 +3179,7 @@
         <v>193</v>
       </c>
       <c r="C100" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -3190,7 +3190,7 @@
         <v>195</v>
       </c>
       <c r="C101" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -3201,7 +3201,7 @@
         <v>197</v>
       </c>
       <c r="C102" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="25.5">
@@ -3212,7 +3212,7 @@
         <v>199</v>
       </c>
       <c r="C103" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -3223,7 +3223,7 @@
         <v>201</v>
       </c>
       <c r="C104" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -3234,7 +3234,7 @@
         <v>203</v>
       </c>
       <c r="C105" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -3245,7 +3245,7 @@
         <v>205</v>
       </c>
       <c r="C106" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -3256,7 +3256,7 @@
         <v>207</v>
       </c>
       <c r="C107" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="25.5">
@@ -3267,7 +3267,7 @@
         <v>209</v>
       </c>
       <c r="C108" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -3278,7 +3278,7 @@
         <v>211</v>
       </c>
       <c r="C109" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -3289,7 +3289,7 @@
         <v>213</v>
       </c>
       <c r="C110" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -3300,7 +3300,7 @@
         <v>215</v>
       </c>
       <c r="C111" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -3311,7 +3311,7 @@
         <v>217</v>
       </c>
       <c r="C112" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -3322,7 +3322,7 @@
         <v>219</v>
       </c>
       <c r="C113" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -3333,7 +3333,7 @@
         <v>221</v>
       </c>
       <c r="C114" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -3344,7 +3344,7 @@
         <v>223</v>
       </c>
       <c r="C115" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -3355,7 +3355,7 @@
         <v>224</v>
       </c>
       <c r="C116" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -3366,7 +3366,7 @@
         <v>226</v>
       </c>
       <c r="C117" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -3377,7 +3377,7 @@
         <v>228</v>
       </c>
       <c r="C118" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -3388,7 +3388,7 @@
         <v>230</v>
       </c>
       <c r="C119" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -3399,7 +3399,7 @@
         <v>232</v>
       </c>
       <c r="C120" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -3410,7 +3410,7 @@
         <v>234</v>
       </c>
       <c r="C121" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -3421,7 +3421,7 @@
         <v>236</v>
       </c>
       <c r="C122" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -3432,7 +3432,7 @@
         <v>238</v>
       </c>
       <c r="C123" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -3443,7 +3443,7 @@
         <v>240</v>
       </c>
       <c r="C124" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -3454,7 +3454,7 @@
         <v>242</v>
       </c>
       <c r="C125" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -3476,7 +3476,7 @@
         <v>246</v>
       </c>
       <c r="C127" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -3487,7 +3487,7 @@
         <v>248</v>
       </c>
       <c r="C128" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -3498,7 +3498,7 @@
         <v>250</v>
       </c>
       <c r="C129" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -3509,7 +3509,7 @@
         <v>252</v>
       </c>
       <c r="C130" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -3520,7 +3520,7 @@
         <v>254</v>
       </c>
       <c r="C131" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -3531,7 +3531,7 @@
         <v>256</v>
       </c>
       <c r="C132" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="25.5">
@@ -3542,7 +3542,7 @@
         <v>258</v>
       </c>
       <c r="C133" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="25.5">
@@ -3553,7 +3553,7 @@
         <v>260</v>
       </c>
       <c r="C134" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -3564,7 +3564,7 @@
         <v>262</v>
       </c>
       <c r="C135" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -3575,7 +3575,7 @@
         <v>264</v>
       </c>
       <c r="C136" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -3586,7 +3586,7 @@
         <v>266</v>
       </c>
       <c r="C137" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -3597,7 +3597,7 @@
         <v>268</v>
       </c>
       <c r="C138" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -3608,7 +3608,7 @@
         <v>270</v>
       </c>
       <c r="C139" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -3619,7 +3619,7 @@
         <v>272</v>
       </c>
       <c r="C140" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -3630,7 +3630,7 @@
         <v>274</v>
       </c>
       <c r="C141" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -3663,7 +3663,7 @@
         <v>277</v>
       </c>
       <c r="C144" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -3674,7 +3674,7 @@
         <v>279</v>
       </c>
       <c r="C145" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -3685,7 +3685,7 @@
         <v>281</v>
       </c>
       <c r="C146" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -3696,7 +3696,7 @@
         <v>283</v>
       </c>
       <c r="C147" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -3707,7 +3707,7 @@
         <v>285</v>
       </c>
       <c r="C148" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -3718,7 +3718,7 @@
         <v>287</v>
       </c>
       <c r="C149" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -3729,7 +3729,7 @@
         <v>289</v>
       </c>
       <c r="C150" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -3740,7 +3740,7 @@
         <v>291</v>
       </c>
       <c r="C151" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -3751,7 +3751,7 @@
         <v>293</v>
       </c>
       <c r="C152" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -3762,7 +3762,7 @@
         <v>295</v>
       </c>
       <c r="C153" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -3773,7 +3773,7 @@
         <v>297</v>
       </c>
       <c r="C154" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -3784,7 +3784,7 @@
         <v>299</v>
       </c>
       <c r="C155" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -3795,7 +3795,7 @@
         <v>301</v>
       </c>
       <c r="C156" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -3806,7 +3806,7 @@
         <v>303</v>
       </c>
       <c r="C157" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -3839,7 +3839,7 @@
         <v>306</v>
       </c>
       <c r="C160" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -3861,7 +3861,7 @@
         <v>309</v>
       </c>
       <c r="C162" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3872,7 +3872,7 @@
         <v>311</v>
       </c>
       <c r="C163" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -3927,7 +3927,7 @@
         <v>318</v>
       </c>
       <c r="C168" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3938,7 +3938,7 @@
         <v>319</v>
       </c>
       <c r="C169" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3949,7 +3949,7 @@
         <v>320</v>
       </c>
       <c r="C170" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3960,7 +3960,7 @@
         <v>321</v>
       </c>
       <c r="C171" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -4114,7 +4114,7 @@
         <v>336</v>
       </c>
       <c r="C185" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -4125,7 +4125,7 @@
         <v>338</v>
       </c>
       <c r="C186" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -4323,7 +4323,7 @@
         <v>373</v>
       </c>
       <c r="C204" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -4334,7 +4334,7 @@
         <v>375</v>
       </c>
       <c r="C205" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -4345,7 +4345,7 @@
         <v>377</v>
       </c>
       <c r="C206" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -4356,7 +4356,7 @@
         <v>379</v>
       </c>
       <c r="C207" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -4367,7 +4367,7 @@
         <v>381</v>
       </c>
       <c r="C208" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -4378,7 +4378,7 @@
         <v>383</v>
       </c>
       <c r="C209" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -4455,7 +4455,7 @@
         <v>396</v>
       </c>
       <c r="C216" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="217" spans="1:3">

</xml_diff>

<commit_message>
Editor respects movement key bindings. WIP wall-run exploit fix and main menu leaderboard view.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="571">
   <si>
     <t>en</t>
   </si>
@@ -994,6 +994,15 @@
   </si>
   <si>
     <t>Znajomi</t>
+  </si>
+  <si>
+    <t>leaderboard title</t>
+  </si>
+  <si>
+    <t>L E A D E R B O A R D</t>
+  </si>
+  <si>
+    <t>R A N K I N G</t>
   </si>
   <si>
     <t>leaderboard</t>
@@ -1843,10 +1852,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3109,7 +3118,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>325</v>
       </c>
@@ -3136,15 +3145,15 @@
         <v>331</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>334</v>
@@ -3249,15 +3258,15 @@
         <v>361</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C128" s="0" t="s">
         <v>364</v>
@@ -3318,7 +3327,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>380</v>
       </c>
@@ -3340,7 +3349,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>386</v>
       </c>
@@ -3422,32 +3431,32 @@
         <v>407</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>47</v>
+        <v>410</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>408</v>
+        <v>46</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>409</v>
+        <v>46</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>410</v>
+        <v>47</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3531,7 +3540,7 @@
       <c r="A153" s="0" t="s">
         <v>432</v>
       </c>
-      <c r="B153" s="0" t="s">
+      <c r="B153" s="1" t="s">
         <v>433</v>
       </c>
       <c r="C153" s="0" t="s">
@@ -3597,60 +3606,60 @@
       <c r="A159" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>450</v>
+      <c r="B159" s="0" t="s">
+        <v>451</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>455</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>459</v>
@@ -3667,238 +3676,238 @@
         <v>462</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>478</v>
-      </c>
-      <c r="B176" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C176" s="0" t="n">
-        <v>0</v>
+        <v>480</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C176" s="0" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B177" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C177" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C178" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C179" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B180" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C180" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B181" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C181" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B182" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C182" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="B183" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C183" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B184" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C184" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B185" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C185" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="C186" s="0" t="s">
         <v>490</v>
+      </c>
+      <c r="B186" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C186" s="0" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3920,191 +3929,191 @@
         <v>495</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C189" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C194" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C197" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="B203" s="0" t="s">
         <v>525</v>
       </c>
+      <c r="B203" s="1" t="s">
+        <v>526</v>
+      </c>
       <c r="C203" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>526</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>528</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C205" s="0" t="s">
         <v>529</v>
@@ -4173,125 +4182,136 @@
         <v>546</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
+      </c>
+      <c r="C217" s="0" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="C218" s="0" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>567</v>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="C223" s="0" t="s">
+        <v>570</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "minimize camera motion" option. Fix menu leaderboard issues. Add player velocity debug display. Update README with Oculus info. Add more build scripts. Bump version number.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="573">
   <si>
     <t>en</t>
   </si>
@@ -472,6 +472,12 @@
   </si>
   <si>
     <t>Zapytaj</t>
+  </si>
+  <si>
+    <t>minimize head bob</t>
+  </si>
+  <si>
+    <t>Minimize camera motion</t>
   </si>
   <si>
     <t>sound effect volume</t>
@@ -1852,10 +1858,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C223"/>
+  <dimension ref="A1:C224"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B29" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2469,7 +2475,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>151</v>
       </c>
@@ -2477,147 +2483,147 @@
         <v>152</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="0" t="s">
         <v>164</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="0" t="s">
         <v>170</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="0" t="s">
         <v>173</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="0" t="s">
         <v>185</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" s="0" t="s">
         <v>188</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>191</v>
@@ -2631,169 +2637,169 @@
         <v>193</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" s="0" t="s">
         <v>196</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="C73" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="C75" s="0" t="s">
         <v>208</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="0" t="s">
         <v>211</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C77" s="0" t="s">
         <v>214</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="C78" s="0" t="s">
         <v>217</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="0" t="s">
         <v>220</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="0" t="s">
         <v>223</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="C81" s="0" t="s">
         <v>226</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C82" s="0" t="s">
         <v>229</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="0" t="s">
         <v>232</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="0" t="s">
         <v>235</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>238</v>
@@ -2807,208 +2813,208 @@
         <v>240</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="C87" s="0" t="s">
         <v>243</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="0" t="s">
         <v>246</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C89" s="0" t="s">
         <v>249</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="C90" s="0" t="s">
         <v>252</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="C91" s="0" t="s">
         <v>255</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="C92" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="C92" s="0" t="s">
+    </row>
+    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="B93" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="C93" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="C93" s="0" t="s">
+    </row>
+    <row r="94" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+      <c r="B94" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="C94" s="0" t="s">
         <v>264</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="C95" s="0" t="s">
         <v>267</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="C96" s="0" t="s">
         <v>270</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="C97" s="0" t="s">
         <v>273</v>
-      </c>
-      <c r="C97" s="0" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="C98" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="C98" s="0" t="s">
+    </row>
+    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="99" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="B99" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="C99" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="C99" s="0" t="s">
+    </row>
+    <row r="100" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+      <c r="B100" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="C100" s="0" t="s">
         <v>282</v>
-      </c>
-      <c r="C100" s="0" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="C101" s="0" t="s">
         <v>285</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="0" t="s">
         <v>288</v>
-      </c>
-      <c r="C102" s="0" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="C103" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="C103" s="0" t="s">
+    </row>
+    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+      <c r="B104" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="C104" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="C104" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="105" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>295</v>
       </c>
@@ -3016,144 +3022,144 @@
         <v>296</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="C106" s="0" t="s">
         <v>299</v>
-      </c>
-      <c r="C106" s="0" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="C107" s="0" t="s">
         <v>302</v>
-      </c>
-      <c r="C107" s="0" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="C108" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="C108" s="0" t="s">
+    </row>
+    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="109" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="B109" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="C109" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="C109" s="0" t="s">
+    </row>
+    <row r="110" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="B110" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="C110" s="0" t="s">
         <v>311</v>
-      </c>
-      <c r="C110" s="0" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="C111" s="0" t="s">
         <v>314</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="C112" s="0" t="s">
         <v>317</v>
-      </c>
-      <c r="C112" s="0" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="C113" s="0" t="s">
         <v>320</v>
-      </c>
-      <c r="C113" s="0" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="C114" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="C114" s="0" t="s">
+    </row>
+    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+      <c r="B115" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="C115" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="C115" s="0" t="s">
+    </row>
+    <row r="116" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+      <c r="B116" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="C116" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="C116" s="0" t="s">
+    </row>
+    <row r="117" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="B117" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="C117" s="0" t="s">
         <v>332</v>
-      </c>
-      <c r="C117" s="0" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>334</v>
@@ -3167,106 +3173,106 @@
         <v>336</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C119" s="0" t="s">
         <v>337</v>
-      </c>
-      <c r="C119" s="0" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="C120" s="0" t="s">
         <v>340</v>
-      </c>
-      <c r="C120" s="0" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="C121" s="0" t="s">
         <v>343</v>
-      </c>
-      <c r="C121" s="0" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="C122" s="0" t="s">
         <v>346</v>
-      </c>
-      <c r="C122" s="0" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="C123" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="C123" s="0" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="C124" s="0" t="s">
         <v>352</v>
-      </c>
-      <c r="C124" s="0" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="C125" s="0" t="s">
         <v>355</v>
-      </c>
-      <c r="C125" s="0" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="C126" s="0" t="s">
         <v>358</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="C127" s="0" t="s">
         <v>361</v>
-      </c>
-      <c r="C127" s="0" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>364</v>
       </c>
       <c r="C128" s="0" t="s">
         <v>364</v>
@@ -3280,367 +3286,367 @@
         <v>366</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="C130" s="0" t="s">
         <v>369</v>
-      </c>
-      <c r="C130" s="0" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="C131" s="0" t="s">
         <v>372</v>
-      </c>
-      <c r="C131" s="0" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="C132" s="0" t="s">
         <v>375</v>
-      </c>
-      <c r="C132" s="0" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="C133" s="0" t="s">
         <v>378</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="C134" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="C134" s="0" t="s">
+    </row>
+    <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="135" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
+      <c r="B135" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="C135" s="0" t="s">
         <v>384</v>
-      </c>
-      <c r="C135" s="0" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="C136" s="0" t="s">
         <v>387</v>
       </c>
-      <c r="C136" s="0" t="s">
+    </row>
+    <row r="137" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
+      <c r="B137" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="C137" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="C137" s="0" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="C138" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="C138" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="C139" s="0" t="s">
         <v>396</v>
-      </c>
-      <c r="C139" s="0" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="C140" s="0" t="s">
         <v>399</v>
-      </c>
-      <c r="C140" s="0" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="C141" s="0" t="s">
         <v>402</v>
-      </c>
-      <c r="C141" s="0" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="C142" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="C142" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="C143" s="0" t="s">
         <v>408</v>
-      </c>
-      <c r="C143" s="0" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>410</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>46</v>
+        <v>412</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>46</v>
+        <v>412</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>47</v>
+        <v>412</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>411</v>
+        <v>46</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>412</v>
+        <v>46</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>413</v>
+        <v>47</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="C147" s="0" t="s">
         <v>415</v>
-      </c>
-      <c r="C147" s="0" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="C148" s="0" t="s">
         <v>418</v>
-      </c>
-      <c r="C148" s="0" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="C149" s="0" t="s">
         <v>421</v>
-      </c>
-      <c r="C149" s="0" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="C150" s="0" t="s">
         <v>424</v>
-      </c>
-      <c r="C150" s="0" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="C151" s="0" t="s">
         <v>427</v>
-      </c>
-      <c r="C151" s="0" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="C152" s="0" t="s">
         <v>430</v>
-      </c>
-      <c r="C152" s="0" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="C153" s="0" t="s">
         <v>433</v>
-      </c>
-      <c r="C153" s="0" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="B154" s="0" t="s">
+      <c r="C154" s="0" t="s">
         <v>436</v>
-      </c>
-      <c r="C154" s="0" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="B155" s="0" t="s">
         <v>438</v>
       </c>
-      <c r="B155" s="0" t="s">
+      <c r="C155" s="0" t="s">
         <v>439</v>
-      </c>
-      <c r="C155" s="0" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="B156" s="0" t="s">
         <v>441</v>
       </c>
-      <c r="B156" s="0" t="s">
+      <c r="C156" s="0" t="s">
         <v>442</v>
-      </c>
-      <c r="C156" s="0" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="B157" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="B157" s="0" t="s">
+      <c r="C157" s="0" t="s">
         <v>445</v>
-      </c>
-      <c r="C157" s="0" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="B158" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="B158" s="0" t="s">
+      <c r="C158" s="0" t="s">
         <v>448</v>
-      </c>
-      <c r="C158" s="0" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="B159" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="B159" s="0" t="s">
+      <c r="C159" s="0" t="s">
         <v>451</v>
-      </c>
-      <c r="C159" s="0" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="B160" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="B160" s="1" t="s">
-        <v>453</v>
-      </c>
       <c r="C160" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C162" s="0" t="s">
         <v>456</v>
@@ -3651,7 +3657,7 @@
         <v>457</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C163" s="0" t="s">
         <v>458</v>
@@ -3662,7 +3668,7 @@
         <v>459</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C164" s="0" t="s">
         <v>460</v>
@@ -3673,18 +3679,18 @@
         <v>461</v>
       </c>
       <c r="B165" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C165" s="0" t="s">
         <v>462</v>
-      </c>
-      <c r="C165" s="0" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>465</v>
       </c>
       <c r="C166" s="0" t="s">
         <v>465</v>
@@ -3706,29 +3712,29 @@
         <v>468</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C170" s="0" t="s">
         <v>471</v>
@@ -3775,169 +3781,169 @@
         <v>478</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="B177" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C177" s="0" t="n">
-        <v>0</v>
+        <v>482</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C178" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C179" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B180" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C180" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B181" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C181" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B182" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C182" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B183" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C183" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B184" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C184" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B185" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C185" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B186" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C186" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="B187" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="C187" s="0" t="s">
-        <v>493</v>
+      <c r="B187" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C187" s="0" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B188" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="B188" s="1" t="s">
+      <c r="C188" s="0" t="s">
         <v>495</v>
-      </c>
-      <c r="C188" s="0" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="B189" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>498</v>
       </c>
       <c r="C189" s="0" t="s">
         <v>498</v>
@@ -4101,7 +4107,7 @@
       <c r="A204" s="0" t="s">
         <v>527</v>
       </c>
-      <c r="B204" s="0" t="s">
+      <c r="B204" s="1" t="s">
         <v>528</v>
       </c>
       <c r="C204" s="0" t="s">
@@ -4112,85 +4118,85 @@
       <c r="A205" s="0" t="s">
         <v>529</v>
       </c>
-      <c r="B205" s="1" t="s">
-        <v>529</v>
+      <c r="B205" s="0" t="s">
+        <v>530</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>531</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="C207" s="0" t="s">
         <v>534</v>
-      </c>
-      <c r="C207" s="0" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
+        <v>535</v>
+      </c>
+      <c r="B208" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="B208" s="1" t="s">
+      <c r="C208" s="0" t="s">
         <v>537</v>
-      </c>
-      <c r="C208" s="0" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="B209" s="1" t="s">
+      <c r="C209" s="0" t="s">
         <v>540</v>
-      </c>
-      <c r="C209" s="0" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="B210" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="B210" s="1" t="s">
+      <c r="C210" s="0" t="s">
         <v>543</v>
-      </c>
-      <c r="C210" s="0" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="C211" s="0" t="s">
         <v>546</v>
-      </c>
-      <c r="C211" s="0" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="B212" s="1" t="s">
         <v>548</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>549</v>
       </c>
       <c r="C212" s="0" t="s">
         <v>549</v>
@@ -4212,21 +4218,21 @@
         <v>552</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4258,6 +4264,9 @@
       <c r="B218" s="1" t="s">
         <v>560</v>
       </c>
+      <c r="C218" s="0" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
@@ -4266,9 +4275,6 @@
       <c r="B219" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="C219" s="0" t="s">
-        <v>562</v>
-      </c>
     </row>
     <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
@@ -4312,6 +4318,17 @@
       </c>
       <c r="C223" s="0" t="s">
         <v>570</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="C224" s="0" t="s">
+        <v>572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add key bind option for console toggle. Fix wall-run exploit for good. Fix challenge menu glitch on workshop maps.
</commit_message>
<xml_diff>
--- a/Lemma/Content/Strings.xlsx
+++ b/Lemma/Content/Strings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="577">
   <si>
     <t>en</t>
   </si>
@@ -480,6 +480,9 @@
     <t>Minimize camera motion</t>
   </si>
   <si>
+    <t>Zmniejsz kołysanie ekranu</t>
+  </si>
+  <si>
     <t>sound effect volume</t>
   </si>
   <si>
@@ -612,6 +615,15 @@
     <t>Obrót / Kopnięcie</t>
   </si>
   <si>
+    <t>toggle console</t>
+  </si>
+  <si>
+    <t>Toggle console</t>
+  </si>
+  <si>
+    <t>Włącz konsolę</t>
+  </si>
+  <si>
     <t>toggle phone</t>
   </si>
   <si>
@@ -1188,10 +1200,10 @@
     <t>god mode</t>
   </si>
   <si>
-    <t>GOD MODE ACTIVATED. Press [~] to toggle console.</t>
-  </si>
-  <si>
-    <t>TRYB BOGA AKTYWOWANY. Naciśnij [~] by włączyć konsolę.</t>
+    <t>GOD MODE ACTIVATED. Press [{{ToggleConsole}}] to toggle console.</t>
+  </si>
+  <si>
+    <t>TRYB BOGA AKTYWOWANY. Naciśnij [{{ToggleConsole}}] by włączyć konsolę.</t>
   </si>
   <si>
     <t>LeftMouseButton</t>
@@ -1858,10 +1870,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B29" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B124" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B139" activeCellId="0" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2483,1852 +2495,1863 @@
         <v>152</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="B100" s="4" t="s">
         <v>281</v>
       </c>
+      <c r="B100" s="1" t="s">
+        <v>282</v>
+      </c>
       <c r="C100" s="0" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="B101" s="1" t="s">
         <v>284</v>
       </c>
+      <c r="B101" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="C101" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>46</v>
+        <v>416</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>46</v>
+        <v>416</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>47</v>
+        <v>416</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>413</v>
+        <v>46</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>414</v>
+        <v>46</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>415</v>
+        <v>47</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>437</v>
-      </c>
-      <c r="B155" s="0" t="s">
         <v>438</v>
       </c>
+      <c r="B155" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="C155" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>455</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>457</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="B178" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C178" s="0" t="n">
-        <v>0</v>
+        <v>486</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C179" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B180" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C180" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B181" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C181" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="B182" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C182" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="B183" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C183" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="B184" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C184" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B185" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C185" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="B186" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C186" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="B187" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C187" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>493</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="C188" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
+      </c>
+      <c r="B188" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C188" s="0" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C189" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C194" s="0" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C197" s="0" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>529</v>
-      </c>
-      <c r="B205" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>531</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>534</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C209" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
+        <v>558</v>
+      </c>
+      <c r="B216" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="B216" s="1" t="s">
-        <v>556</v>
-      </c>
       <c r="C216" s="0" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>562</v>
+        <v>564</v>
+      </c>
+      <c r="C219" s="0" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="C220" s="0" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
+        <v>575</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C225" s="0" t="s">
+        <v>576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>